<commit_message>
Deleted a wrong link
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="154">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -356,10 +356,6 @@
   </si>
   <si>
     <t>US substitution</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Amazon.com</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1006,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1019,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1035,21 +1031,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1063,7 +1059,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1077,7 +1073,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1091,7 +1087,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1105,7 +1101,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1119,7 +1115,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1133,7 +1129,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1147,7 +1143,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1161,7 +1157,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1175,7 +1171,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1189,7 +1185,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1203,7 +1199,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1217,7 +1213,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1231,7 +1227,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1245,7 +1241,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1259,7 +1255,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1273,7 +1269,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1287,7 +1283,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1301,7 +1297,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1315,7 +1311,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1329,7 +1325,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1343,7 +1339,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1357,7 +1353,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1371,7 +1367,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1385,7 +1381,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1399,7 +1395,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -1413,7 +1409,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1427,7 +1423,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1441,7 +1437,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1455,7 +1451,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1469,7 +1465,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1483,7 +1479,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -1497,7 +1493,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1511,7 +1507,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1525,7 +1521,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1539,7 +1535,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1553,7 +1549,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1567,7 +1563,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1581,7 +1577,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1595,7 +1591,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1609,7 +1605,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1623,7 +1619,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1637,7 +1633,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1651,7 +1647,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -1665,7 +1661,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1679,7 +1675,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -1700,7 +1696,7 @@
     </row>
     <row r="48" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -1717,13 +1713,13 @@
     </row>
     <row r="49" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1734,30 +1730,30 @@
     </row>
     <row r="50" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1768,7 +1764,7 @@
     </row>
     <row r="52" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
@@ -1785,7 +1781,7 @@
     </row>
     <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
         <v>66</v>
@@ -1802,13 +1798,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" t="s">
         <v>92</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -1816,22 +1812,20 @@
       <c r="E54" t="s">
         <v>84</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="1"/>
+      <c r="G54" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1840,35 +1834,35 @@
         <v>87</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="E56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="D57">
         <v>14</v>
@@ -1879,13 +1873,13 @@
     </row>
     <row r="58" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1896,13 +1890,13 @@
     </row>
     <row r="59" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -1913,30 +1907,30 @@
     </row>
     <row r="60" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D60">
         <v>6</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D61">
         <v>12</v>
@@ -1947,41 +1941,41 @@
     </row>
     <row r="62" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D62">
         <v>9</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D63">
         <v>7</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
         <v>55</v>
@@ -1995,13 +1989,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2009,7 +2003,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2030,7 +2024,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
@@ -2041,7 +2035,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B70" t="s">
         <v>82</v>
@@ -2061,7 +2055,7 @@
     </row>
     <row r="71" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
@@ -2082,7 +2076,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
@@ -2100,7 +2094,7 @@
     </row>
     <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
@@ -2119,7 +2113,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
@@ -2137,7 +2131,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B75" t="s">
         <v>85</v>
@@ -2155,7 +2149,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B76" t="s">
         <v>88</v>
@@ -2176,44 +2170,44 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D77">
         <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>141</v>
+      </c>
+      <c r="B80" t="s">
         <v>142</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>143</v>
-      </c>
-      <c r="C80" t="s">
-        <v>144</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -2221,10 +2215,10 @@
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>77</v>
@@ -2238,30 +2232,30 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B82" t="s">
+        <v>145</v>
+      </c>
+      <c r="C82" t="s">
         <v>146</v>
       </c>
-      <c r="C82" t="s">
-        <v>147</v>
-      </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B83" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -2269,13 +2263,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B84" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2283,22 +2277,22 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B85" t="s">
+        <v>151</v>
+      </c>
+      <c r="C85" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C85" t="s">
-        <v>151</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H85" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2321,31 +2315,30 @@
     <hyperlink ref="E75" r:id="rId15"/>
     <hyperlink ref="E76" r:id="rId16"/>
     <hyperlink ref="G76" r:id="rId17"/>
-    <hyperlink ref="F54" r:id="rId18"/>
-    <hyperlink ref="G54" r:id="rId19"/>
-    <hyperlink ref="E55" r:id="rId20"/>
-    <hyperlink ref="G55" r:id="rId21"/>
-    <hyperlink ref="G56" r:id="rId22"/>
-    <hyperlink ref="E56" r:id="rId23"/>
-    <hyperlink ref="E77" r:id="rId24"/>
-    <hyperlink ref="G77" r:id="rId25"/>
-    <hyperlink ref="G78" r:id="rId26"/>
-    <hyperlink ref="G57" r:id="rId27"/>
-    <hyperlink ref="G58" r:id="rId28"/>
-    <hyperlink ref="G60" r:id="rId29" display="wilco"/>
-    <hyperlink ref="G61" r:id="rId30"/>
-    <hyperlink ref="G62" r:id="rId31" display="wilco"/>
-    <hyperlink ref="G63" r:id="rId32" display="wilco"/>
-    <hyperlink ref="G50" r:id="rId33"/>
-    <hyperlink ref="G59" r:id="rId34"/>
-    <hyperlink ref="G49" r:id="rId35"/>
-    <hyperlink ref="G81" r:id="rId36"/>
-    <hyperlink ref="G82" r:id="rId37"/>
-    <hyperlink ref="E85" r:id="rId38"/>
-    <hyperlink ref="H85" r:id="rId39"/>
+    <hyperlink ref="G54" r:id="rId18"/>
+    <hyperlink ref="E55" r:id="rId19"/>
+    <hyperlink ref="G55" r:id="rId20"/>
+    <hyperlink ref="G56" r:id="rId21"/>
+    <hyperlink ref="E56" r:id="rId22"/>
+    <hyperlink ref="E77" r:id="rId23"/>
+    <hyperlink ref="G77" r:id="rId24"/>
+    <hyperlink ref="G78" r:id="rId25"/>
+    <hyperlink ref="G57" r:id="rId26"/>
+    <hyperlink ref="G58" r:id="rId27"/>
+    <hyperlink ref="G60" r:id="rId28" display="wilco"/>
+    <hyperlink ref="G61" r:id="rId29"/>
+    <hyperlink ref="G62" r:id="rId30" display="wilco"/>
+    <hyperlink ref="G63" r:id="rId31" display="wilco"/>
+    <hyperlink ref="G50" r:id="rId32"/>
+    <hyperlink ref="G59" r:id="rId33"/>
+    <hyperlink ref="G49" r:id="rId34"/>
+    <hyperlink ref="G81" r:id="rId35"/>
+    <hyperlink ref="G82" r:id="rId36"/>
+    <hyperlink ref="E85" r:id="rId37"/>
+    <hyperlink ref="H85" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added the link to a substitution of small servo motor
Emax ES08MD
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="155">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -630,6 +630,10 @@
   </si>
   <si>
     <t>*TBD*</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon.com</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1002,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1816,9 @@
       <c r="E54" t="s">
         <v>84</v>
       </c>
-      <c r="F54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>94</v>
       </c>
@@ -2336,9 +2342,10 @@
     <hyperlink ref="G82" r:id="rId36"/>
     <hyperlink ref="E85" r:id="rId37"/>
     <hyperlink ref="H85" r:id="rId38"/>
+    <hyperlink ref="F54" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId40"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the substitution link of the battery.
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="159">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -634,6 +634,22 @@
   </si>
   <si>
     <t>Amazon.com</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon.com</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NA</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1006,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1481,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>136</v>
       </c>
@@ -1495,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>136</v>
       </c>
@@ -1509,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -1523,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>136</v>
       </c>
@@ -1537,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>136</v>
       </c>
@@ -1551,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>136</v>
       </c>
@@ -1565,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -1579,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -1593,7 +1609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -1607,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -1621,7 +1637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -1635,7 +1651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -1649,7 +1665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -1663,7 +1679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>136</v>
       </c>
@@ -1677,7 +1693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>136</v>
       </c>
@@ -1693,12 +1709,17 @@
       <c r="E47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="G47" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>136</v>
       </c>
@@ -2053,10 +2074,10 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="G70" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
@@ -2217,6 +2238,12 @@
       </c>
       <c r="D80">
         <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>158</v>
+      </c>
+      <c r="G80" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
@@ -2343,9 +2370,11 @@
     <hyperlink ref="E85" r:id="rId37"/>
     <hyperlink ref="H85" r:id="rId38"/>
     <hyperlink ref="F54" r:id="rId39"/>
+    <hyperlink ref="H47" r:id="rId40"/>
+    <hyperlink ref="F47" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId42"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Upgraded the strength of index finger
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -416,17 +416,6 @@
   </si>
   <si>
     <t>marutu</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ScrewM2L8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Tapping screw
--Shaft diameter:2
--Head diameter:3.5
--Length:8</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -650,6 +639,17 @@
   </si>
   <si>
     <t>NA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ScrewM2L10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tapping screw
+-Shaft diameter:2
+-Head diameter:3.5
+-Length:10</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1039,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1051,21 +1051,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -1710,18 +1710,18 @@
         <v>50</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -1738,13 +1738,13 @@
     </row>
     <row r="49" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1755,30 +1755,30 @@
     </row>
     <row r="50" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="52" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
         <v>66</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B54" t="s">
         <v>92</v>
@@ -1838,7 +1838,7 @@
         <v>84</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>94</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B55" t="s">
         <v>95</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="56" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
         <v>99</v>
@@ -1883,13 +1883,13 @@
     </row>
     <row r="57" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="D57">
         <v>14</v>
@@ -1900,13 +1900,13 @@
     </row>
     <row r="58" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1917,13 +1917,13 @@
     </row>
     <row r="59" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -1934,30 +1934,30 @@
     </row>
     <row r="60" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D60">
         <v>6</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D61">
         <v>12</v>
@@ -1968,41 +1968,41 @@
     </row>
     <row r="62" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D62">
         <v>9</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D63">
         <v>7</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B65" t="s">
         <v>55</v>
@@ -2016,13 +2016,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B70" t="s">
         <v>82</v>
@@ -2074,15 +2074,15 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G70" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B75" t="s">
         <v>85</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B76" t="s">
         <v>88</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B77" t="s">
         <v>103</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B78" t="s">
         <v>106</v>
@@ -2228,30 +2228,30 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" t="s">
+        <v>140</v>
+      </c>
+      <c r="C80" t="s">
         <v>141</v>
       </c>
-      <c r="B80" t="s">
-        <v>142</v>
-      </c>
-      <c r="C80" t="s">
-        <v>143</v>
-      </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G80" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B81" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>77</v>
@@ -2265,30 +2265,30 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B82" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C82" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B83" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C83" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -2296,13 +2296,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C84" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2310,22 +2310,22 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B85" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C85" t="s">
+        <v>148</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="H85" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added minor errors of BOM
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="162">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -554,10 +554,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MC2374L</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DC Plug</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -650,6 +646,22 @@
 -Shaft diameter:2
 -Head diameter:3.5
 -Length:10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Slide Switch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>momohara</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MC2374L</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mouser</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1022,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1710,13 +1722,13 @@
         <v>50</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
@@ -1838,7 +1850,7 @@
         <v>84</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>94</v>
@@ -1874,6 +1886,9 @@
       <c r="C56" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
       <c r="E56" s="1" t="s">
         <v>102</v>
       </c>
@@ -1886,10 +1901,10 @@
         <v>134</v>
       </c>
       <c r="B57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="D57">
         <v>14</v>
@@ -2002,7 +2017,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
         <v>55</v>
@@ -2016,21 +2031,27 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B66" t="s">
+        <v>160</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="D66">
         <v>1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2051,7 +2072,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
@@ -2059,10 +2080,16 @@
       <c r="C68" t="s">
         <v>56</v>
       </c>
+      <c r="E68" t="s">
+        <v>154</v>
+      </c>
+      <c r="G68" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
         <v>82</v>
@@ -2074,15 +2101,15 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
@@ -2103,7 +2130,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
@@ -2121,7 +2148,7 @@
     </row>
     <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
@@ -2140,7 +2167,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
@@ -2158,7 +2185,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
         <v>85</v>
@@ -2176,7 +2203,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B76" t="s">
         <v>88</v>
@@ -2197,7 +2224,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B77" t="s">
         <v>103</v>
@@ -2214,11 +2241,14 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B78" t="s">
         <v>106</v>
       </c>
+      <c r="C78" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="D78">
         <v>1</v>
       </c>
@@ -2228,30 +2258,30 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" t="s">
         <v>139</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>140</v>
       </c>
-      <c r="C80" t="s">
-        <v>141</v>
-      </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>77</v>
@@ -2265,30 +2295,30 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B82" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82" t="s">
         <v>143</v>
       </c>
-      <c r="C82" t="s">
-        <v>144</v>
-      </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B83" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -2296,13 +2326,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B84" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2310,22 +2340,22 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B85" t="s">
+        <v>148</v>
+      </c>
+      <c r="C85" t="s">
+        <v>147</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C85" t="s">
-        <v>148</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="H85" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2372,9 +2402,11 @@
     <hyperlink ref="F54" r:id="rId39"/>
     <hyperlink ref="H47" r:id="rId40"/>
     <hyperlink ref="F47" r:id="rId41"/>
+    <hyperlink ref="G66" r:id="rId42"/>
+    <hyperlink ref="F66" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId44"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed the error of the screw length
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -524,17 +524,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>flatScrewM2L4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Flat screw
--Shaft diameter:2
--Head diameter:4
--Length:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>TS 0.4-3.2-14</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -662,6 +651,17 @@
   </si>
   <si>
     <t>mouser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>flatScrewM2L6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Flat screw
+-Shaft diameter:2
+-Head diameter:4
+-Length:6</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -1722,18 +1722,18 @@
         <v>50</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -1750,13 +1750,13 @@
     </row>
     <row r="49" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="50" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B50" t="s">
         <v>123</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="51" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B51" t="s">
         <v>121</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="52" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B53" t="s">
         <v>66</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B54" t="s">
         <v>92</v>
@@ -1850,7 +1850,7 @@
         <v>84</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>94</v>
@@ -1858,7 +1858,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B55" t="s">
         <v>95</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="56" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B56" t="s">
         <v>99</v>
@@ -1898,13 +1898,13 @@
     </row>
     <row r="57" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B57" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D57">
         <v>14</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="58" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B58" t="s">
         <v>108</v>
@@ -1932,13 +1932,13 @@
     </row>
     <row r="59" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="60" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B60" t="s">
         <v>110</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="61" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
         <v>111</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="62" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>115</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="63" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>116</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
         <v>55</v>
@@ -2031,27 +2031,27 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
@@ -2081,15 +2081,15 @@
         <v>56</v>
       </c>
       <c r="E68" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G68" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B70" t="s">
         <v>82</v>
@@ -2101,15 +2101,15 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G70" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
         <v>85</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
         <v>88</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B77" t="s">
         <v>103</v>
@@ -2241,13 +2241,13 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B78" t="s">
         <v>106</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -2258,30 +2258,30 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>136</v>
+      </c>
+      <c r="B80" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" t="s">
         <v>138</v>
       </c>
-      <c r="B80" t="s">
-        <v>139</v>
-      </c>
-      <c r="C80" t="s">
-        <v>140</v>
-      </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G80" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B81" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>77</v>
@@ -2295,30 +2295,30 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B82" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C82" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B83" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C83" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -2326,13 +2326,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B84" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C84" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2340,22 +2340,22 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B85" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C85" t="s">
+        <v>145</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="H85" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the small servo and fixed minor errors.
Changed ASV-15MG to ES08MD.
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -319,10 +319,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>pin header 3 3Pin</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -348,10 +344,6 @@
   </si>
   <si>
     <t>momohara</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ASV-15MG</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -662,6 +654,14 @@
 -Shaft diameter:2
 -Head diameter:4
 -Length:6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ES08MD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon.jp</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1063,21 +1063,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -1722,18 +1722,18 @@
         <v>50</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -1748,15 +1748,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1765,32 +1765,32 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -1799,9 +1799,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
@@ -1816,9 +1816,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
         <v>66</v>
@@ -1833,78 +1833,78 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D54">
         <v>2</v>
       </c>
-      <c r="E54" t="s">
-        <v>84</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>149</v>
+      <c r="E54" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B55" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" t="s">
         <v>97</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G55" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>132</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B57" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D57">
         <v>14</v>
@@ -1913,15 +1913,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1930,15 +1930,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -1947,32 +1947,32 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D60">
         <v>6</v>
       </c>
       <c r="G60" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>132</v>
-      </c>
-      <c r="B61" t="s">
-        <v>111</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D61">
         <v>12</v>
@@ -1981,43 +1981,43 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D62">
         <v>9</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D63">
         <v>7</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B65" t="s">
         <v>55</v>
@@ -2031,27 +2031,27 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D66">
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B68" t="s">
         <v>55</v>
@@ -2081,15 +2081,15 @@
         <v>56</v>
       </c>
       <c r="E68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G68" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B70" t="s">
         <v>82</v>
@@ -2101,15 +2101,15 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G70" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
@@ -2185,103 +2185,103 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B75" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D75">
         <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D77">
         <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D78">
         <v>1</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>134</v>
+      </c>
+      <c r="B80" t="s">
+        <v>135</v>
+      </c>
+      <c r="C80" t="s">
         <v>136</v>
       </c>
-      <c r="B80" t="s">
-        <v>137</v>
-      </c>
-      <c r="C80" t="s">
-        <v>138</v>
-      </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G80" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B81" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>77</v>
@@ -2295,30 +2295,30 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B82" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C82" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B83" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C83" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -2326,13 +2326,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B84" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C84" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2340,22 +2340,22 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B85" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C85" t="s">
+        <v>143</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="H85" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2378,7 +2378,7 @@
     <hyperlink ref="E75" r:id="rId15"/>
     <hyperlink ref="E76" r:id="rId16"/>
     <hyperlink ref="G76" r:id="rId17"/>
-    <hyperlink ref="G54" r:id="rId18"/>
+    <hyperlink ref="H54" r:id="rId18"/>
     <hyperlink ref="E55" r:id="rId19"/>
     <hyperlink ref="G55" r:id="rId20"/>
     <hyperlink ref="G56" r:id="rId21"/>
@@ -2399,14 +2399,15 @@
     <hyperlink ref="G82" r:id="rId36"/>
     <hyperlink ref="E85" r:id="rId37"/>
     <hyperlink ref="H85" r:id="rId38"/>
-    <hyperlink ref="F54" r:id="rId39"/>
+    <hyperlink ref="E54" r:id="rId39"/>
     <hyperlink ref="H47" r:id="rId40"/>
     <hyperlink ref="F47" r:id="rId41"/>
     <hyperlink ref="G66" r:id="rId42"/>
     <hyperlink ref="F66" r:id="rId43"/>
+    <hyperlink ref="G54" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId44"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added the url for a spring store
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$85</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -662,6 +665,24 @@
   </si>
   <si>
     <t>Amazon.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lee Spring
+[LCM050C 02 M]
+*haven't tested yet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lee Spring
+[LE 014A 02 S]
+*haven't tested yet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lee Spring
+[LTL012A 05 M]
+*haven't tested yet</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -710,7 +731,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -718,18 +739,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -1034,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1050,1311 +1090,1616 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
+      <c r="C4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
+      <c r="C6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
+      <c r="C7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
+      <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
+      <c r="C11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
+      <c r="C12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
+      <c r="C13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>130</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>130</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>130</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C32" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
+      <c r="C32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="A33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
+      <c r="C33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="A34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
+      <c r="C34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>130</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="A35" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
+      <c r="C35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="A36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
+      <c r="C36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>130</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="A37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
+      <c r="C37" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>130</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="A38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
+      <c r="C38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>130</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="A39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
+      <c r="C39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>130</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="A40" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
+      <c r="C40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="A41" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C41" t="s">
-        <v>62</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
+      <c r="C41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="A42" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42">
+      <c r="C42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="2">
         <v>3</v>
       </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="A43" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43">
+      <c r="C43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="2">
         <v>3</v>
       </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="A44" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44">
+      <c r="C44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="2">
         <v>3</v>
       </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>130</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="A45" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45">
+      <c r="C45" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="2">
         <v>3</v>
       </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>130</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="A46" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C46" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46">
+      <c r="C46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="2">
         <v>3</v>
       </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>130</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="A47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>130</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="A48" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="2">
         <v>5</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="E48" s="2"/>
+      <c r="F48" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>130</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="A49" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>130</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="A50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="2">
         <v>5</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="E50" s="2"/>
+      <c r="F50" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>130</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="A51" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="2">
         <v>2</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>130</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="A52" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="2">
         <v>6</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>130</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="A53" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="2">
         <v>6</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="A54" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="2">
         <v>2</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="F54" s="2"/>
+      <c r="G54" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>130</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="A55" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="F55" s="2"/>
+      <c r="G55" s="3" t="s">
         <v>96</v>
       </c>
+      <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>130</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="A56" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1" t="s">
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="F56" s="2"/>
+      <c r="G56" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>130</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="A57" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="2">
         <v>14</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>130</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="A58" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1" t="s">
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>130</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="A59" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="2">
         <v>4</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>130</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="A60" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="2">
         <v>6</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="3" t="s">
         <v>110</v>
       </c>
+      <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>130</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="A61" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="2">
         <v>12</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>130</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="A62" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="2">
         <v>9</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>130</v>
-      </c>
-      <c r="B63" s="2" t="s">
+      <c r="A63" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="2">
         <v>7</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="D65" s="2">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="F66" s="1" t="s">
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="G66" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="2">
         <v>2</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1" t="s">
+      <c r="F67" s="3"/>
+      <c r="G67" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E68" t="s">
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G68" t="s">
+      <c r="F68" s="2"/>
+      <c r="G68" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G70" t="s">
+      <c r="F70" s="2"/>
+      <c r="G70" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71" s="1" t="s">
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1" t="s">
+      <c r="F71" s="3"/>
+      <c r="G71" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="E72" s="1" t="s">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1" t="s">
+      <c r="F72" s="3"/>
+      <c r="G72" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1" t="s">
+      <c r="D73" s="2">
+        <v>1</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="2">
         <v>2</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="F74" s="3"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="2">
         <v>5</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="F75" s="3"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76" s="1" t="s">
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1" t="s">
+      <c r="F76" s="3"/>
+      <c r="G76" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D77">
+      <c r="C77" s="2"/>
+      <c r="D77" s="2">
         <v>4</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="F77" s="2"/>
+      <c r="G77" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="G78" s="1" t="s">
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G80" t="s">
+      <c r="F80" s="2"/>
+      <c r="G80" s="2" t="s">
         <v>151</v>
       </c>
+      <c r="H80" s="2"/>
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-      <c r="G81" s="1" t="s">
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D82">
-        <v>1</v>
-      </c>
-      <c r="G82" s="1" t="s">
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="3" t="s">
         <v>142</v>
       </c>
+      <c r="H82" s="2"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D83">
-        <v>1</v>
-      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D84">
-        <v>1</v>
-      </c>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" s="1" t="s">
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H85" s="1" t="s">
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="3" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2405,9 +2750,12 @@
     <hyperlink ref="G66" r:id="rId42"/>
     <hyperlink ref="F66" r:id="rId43"/>
     <hyperlink ref="G54" r:id="rId44"/>
+    <hyperlink ref="F50" r:id="rId45" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
+    <hyperlink ref="F49" r:id="rId46" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
+    <hyperlink ref="F48" r:id="rId47" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
+  <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId48"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the link of steel ball
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="166">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -209,10 +209,6 @@
   </si>
   <si>
     <t>sotec</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>misumi</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -478,10 +474,6 @@
     <t>Shaft
 -Diameter:2
 -Length:15</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SBI-SUJ-1d4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -683,6 +675,18 @@
     <t>Lee Spring
 [LTL012A 05 M]
 *haven't tested yet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SBI-SUJ-1d4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon.jp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon.com</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1075,8 +1079,8 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1096,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1104,27 +1108,27 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -1136,13 +1140,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -1154,13 +1158,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -1172,13 +1176,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1190,13 +1194,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1208,13 +1212,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1226,13 +1230,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -1244,13 +1248,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -1262,13 +1266,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1280,13 +1284,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1298,13 +1302,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1316,13 +1320,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -1334,13 +1338,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -1352,13 +1356,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -1370,13 +1374,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1388,13 +1392,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -1406,13 +1410,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -1424,13 +1428,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -1442,13 +1446,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1460,13 +1464,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1478,13 +1482,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -1496,13 +1500,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
@@ -1514,13 +1518,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -1532,13 +1536,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -1550,13 +1554,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -1568,13 +1572,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -1586,13 +1590,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
@@ -1604,13 +1608,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -1622,13 +1626,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
@@ -1640,13 +1644,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
@@ -1658,13 +1662,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
@@ -1676,13 +1680,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="2">
         <v>1</v>
@@ -1694,13 +1698,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D34" s="2">
         <v>1</v>
@@ -1712,13 +1716,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="2">
         <v>1</v>
@@ -1730,13 +1734,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D36" s="2">
         <v>1</v>
@@ -1748,13 +1752,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="2">
         <v>1</v>
@@ -1766,13 +1770,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D38" s="2">
         <v>1</v>
@@ -1784,13 +1788,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39" s="2">
         <v>1</v>
@@ -1802,13 +1806,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -1820,13 +1824,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -1838,13 +1842,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D42" s="2">
         <v>3</v>
@@ -1856,13 +1860,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43" s="2">
         <v>3</v>
@@ -1874,13 +1878,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44" s="2">
         <v>3</v>
@@ -1892,13 +1896,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D45" s="2">
         <v>3</v>
@@ -1910,13 +1914,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D46" s="2">
         <v>3</v>
@@ -1928,7 +1932,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>49</v>
@@ -1943,31 +1947,31 @@
         <v>50</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>51</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D48" s="2">
         <v>5</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>58</v>
@@ -1976,20 +1980,20 @@
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D49" s="2">
         <v>1</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>58</v>
@@ -1998,55 +2002,57 @@
     </row>
     <row r="50" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D50" s="2">
         <v>5</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="F51" s="2"/>
       <c r="G51" s="3" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="2">
         <v>6</v>
@@ -2054,19 +2060,19 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D53" s="2">
         <v>6</v>
@@ -2074,87 +2080,87 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D54" s="2">
         <v>2</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D55" s="2">
         <v>1</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="D56" s="2">
         <v>1</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D57" s="2">
         <v>14</v>
@@ -2162,19 +2168,19 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
@@ -2182,19 +2188,19 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H58" s="2"/>
     </row>
     <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D59" s="2">
         <v>4</v>
@@ -2202,19 +2208,19 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H59" s="2"/>
     </row>
     <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D60" s="2">
         <v>6</v>
@@ -2222,19 +2228,19 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D61" s="2">
         <v>12</v>
@@ -2242,19 +2248,19 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H61" s="2"/>
     </row>
     <row r="62" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D62" s="2">
         <v>9</v>
@@ -2262,19 +2268,19 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D63" s="2">
         <v>7</v>
@@ -2282,7 +2288,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H63" s="2"/>
     </row>
@@ -2298,7 +2304,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>55</v>
@@ -2316,35 +2322,35 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D67" s="2">
         <v>2</v>
@@ -2360,7 +2366,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>55</v>
@@ -2370,11 +2376,11 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H68" s="2"/>
     </row>
@@ -2390,77 +2396,77 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="D70" s="2">
         <v>1</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="D71" s="2">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H71" s="2"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2">
         <v>1</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="D73" s="2">
         <v>1</v>
@@ -2468,25 +2474,25 @@
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H73" s="2"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D74" s="2">
         <v>2</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="2"/>
@@ -2494,19 +2500,19 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="D75" s="2">
         <v>5</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="2"/>
@@ -2514,55 +2520,55 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D76" s="2">
-        <v>1</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2">
         <v>4</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D78" s="2">
         <v>1</v>
@@ -2570,7 +2576,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H78" s="2"/>
     </row>
@@ -2586,35 +2592,35 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="D80" s="2">
         <v>1</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H80" s="2"/>
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
@@ -2622,19 +2628,19 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
@@ -2642,19 +2648,19 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H82" s="2"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
@@ -2666,13 +2672,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
@@ -2684,24 +2690,24 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="D85" s="2">
-        <v>1</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2712,51 +2718,52 @@
     <hyperlink ref="G67" r:id="rId3"/>
     <hyperlink ref="E67" r:id="rId4"/>
     <hyperlink ref="G48" r:id="rId5" location="prettyphoto/27/"/>
-    <hyperlink ref="G51" r:id="rId6"/>
-    <hyperlink ref="G52" r:id="rId7"/>
-    <hyperlink ref="G53" r:id="rId8"/>
-    <hyperlink ref="G71" r:id="rId9"/>
-    <hyperlink ref="E71" r:id="rId10"/>
-    <hyperlink ref="G72" r:id="rId11"/>
-    <hyperlink ref="E72" r:id="rId12"/>
-    <hyperlink ref="G73" r:id="rId13"/>
-    <hyperlink ref="E74" r:id="rId14"/>
-    <hyperlink ref="E75" r:id="rId15"/>
-    <hyperlink ref="E76" r:id="rId16"/>
-    <hyperlink ref="G76" r:id="rId17"/>
-    <hyperlink ref="H54" r:id="rId18"/>
-    <hyperlink ref="E55" r:id="rId19"/>
-    <hyperlink ref="G55" r:id="rId20"/>
-    <hyperlink ref="G56" r:id="rId21"/>
-    <hyperlink ref="E56" r:id="rId22"/>
-    <hyperlink ref="E77" r:id="rId23"/>
-    <hyperlink ref="G77" r:id="rId24"/>
-    <hyperlink ref="G78" r:id="rId25"/>
-    <hyperlink ref="G57" r:id="rId26"/>
-    <hyperlink ref="G58" r:id="rId27"/>
-    <hyperlink ref="G60" r:id="rId28" display="wilco"/>
-    <hyperlink ref="G61" r:id="rId29"/>
-    <hyperlink ref="G62" r:id="rId30" display="wilco"/>
-    <hyperlink ref="G63" r:id="rId31" display="wilco"/>
-    <hyperlink ref="G50" r:id="rId32"/>
-    <hyperlink ref="G59" r:id="rId33"/>
-    <hyperlink ref="G49" r:id="rId34"/>
-    <hyperlink ref="G81" r:id="rId35"/>
-    <hyperlink ref="G82" r:id="rId36"/>
-    <hyperlink ref="E85" r:id="rId37"/>
-    <hyperlink ref="H85" r:id="rId38"/>
-    <hyperlink ref="E54" r:id="rId39"/>
-    <hyperlink ref="H47" r:id="rId40"/>
-    <hyperlink ref="F47" r:id="rId41"/>
-    <hyperlink ref="G66" r:id="rId42"/>
-    <hyperlink ref="F66" r:id="rId43"/>
-    <hyperlink ref="G54" r:id="rId44"/>
-    <hyperlink ref="F50" r:id="rId45" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
-    <hyperlink ref="F49" r:id="rId46" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
-    <hyperlink ref="F48" r:id="rId47" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
+    <hyperlink ref="G52" r:id="rId6"/>
+    <hyperlink ref="G53" r:id="rId7"/>
+    <hyperlink ref="G71" r:id="rId8"/>
+    <hyperlink ref="E71" r:id="rId9"/>
+    <hyperlink ref="G72" r:id="rId10"/>
+    <hyperlink ref="E72" r:id="rId11"/>
+    <hyperlink ref="G73" r:id="rId12"/>
+    <hyperlink ref="E74" r:id="rId13"/>
+    <hyperlink ref="E75" r:id="rId14"/>
+    <hyperlink ref="E76" r:id="rId15"/>
+    <hyperlink ref="G76" r:id="rId16"/>
+    <hyperlink ref="H54" r:id="rId17"/>
+    <hyperlink ref="E55" r:id="rId18"/>
+    <hyperlink ref="G55" r:id="rId19"/>
+    <hyperlink ref="G56" r:id="rId20"/>
+    <hyperlink ref="E56" r:id="rId21"/>
+    <hyperlink ref="E77" r:id="rId22"/>
+    <hyperlink ref="G77" r:id="rId23"/>
+    <hyperlink ref="G78" r:id="rId24"/>
+    <hyperlink ref="G57" r:id="rId25"/>
+    <hyperlink ref="G58" r:id="rId26"/>
+    <hyperlink ref="G60" r:id="rId27" display="wilco"/>
+    <hyperlink ref="G61" r:id="rId28"/>
+    <hyperlink ref="G62" r:id="rId29" display="wilco"/>
+    <hyperlink ref="G63" r:id="rId30" display="wilco"/>
+    <hyperlink ref="G50" r:id="rId31"/>
+    <hyperlink ref="G59" r:id="rId32"/>
+    <hyperlink ref="G49" r:id="rId33"/>
+    <hyperlink ref="G81" r:id="rId34"/>
+    <hyperlink ref="G82" r:id="rId35"/>
+    <hyperlink ref="E85" r:id="rId36"/>
+    <hyperlink ref="H85" r:id="rId37"/>
+    <hyperlink ref="E54" r:id="rId38"/>
+    <hyperlink ref="H47" r:id="rId39"/>
+    <hyperlink ref="F47" r:id="rId40"/>
+    <hyperlink ref="G66" r:id="rId41"/>
+    <hyperlink ref="F66" r:id="rId42"/>
+    <hyperlink ref="G54" r:id="rId43"/>
+    <hyperlink ref="F50" r:id="rId44" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
+    <hyperlink ref="F49" r:id="rId45" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
+    <hyperlink ref="F48" r:id="rId46" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
+    <hyperlink ref="G51" r:id="rId47"/>
+    <hyperlink ref="E51" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId48"/>
+  <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId49"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed minor URL error
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$85</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$86</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="170">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -302,10 +302,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2.54mm Female Header 1x17</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Pololu</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -338,10 +334,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>PCB Socket</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>momohara</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -363,10 +355,6 @@
   </si>
   <si>
     <t>Servo motor(large)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Akizukidenshi</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -687,6 +675,34 @@
   </si>
   <si>
     <t>Amazon.com</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DC Jack</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tace Switch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Akizuki</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.54mm Female Header 1x10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.54mm Female Header 1x4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pololu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Akizuki</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1076,11 +1092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1112,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1108,21 +1124,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1140,7 +1156,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1158,7 +1174,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1176,7 +1192,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1194,7 +1210,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1212,7 +1228,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -1230,7 +1246,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1248,7 +1264,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
@@ -1266,7 +1282,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
@@ -1284,7 +1300,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -1302,7 +1318,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
@@ -1320,7 +1336,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>14</v>
@@ -1338,7 +1354,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -1356,7 +1372,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1374,7 +1390,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>17</v>
@@ -1392,7 +1408,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
@@ -1410,7 +1426,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
@@ -1428,7 +1444,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
@@ -1446,7 +1462,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
@@ -1464,7 +1480,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
@@ -1482,7 +1498,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -1500,7 +1516,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -1518,7 +1534,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
@@ -1536,7 +1552,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>26</v>
@@ -1554,7 +1570,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>27</v>
@@ -1572,7 +1588,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>28</v>
@@ -1590,7 +1606,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
@@ -1608,7 +1624,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>30</v>
@@ -1626,7 +1642,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>31</v>
@@ -1644,7 +1660,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>32</v>
@@ -1662,7 +1678,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>33</v>
@@ -1680,7 +1696,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>34</v>
@@ -1698,7 +1714,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>35</v>
@@ -1716,7 +1732,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>36</v>
@@ -1734,7 +1750,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>37</v>
@@ -1752,7 +1768,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>38</v>
@@ -1770,7 +1786,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>39</v>
@@ -1788,7 +1804,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>40</v>
@@ -1806,7 +1822,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>41</v>
@@ -1824,7 +1840,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>42</v>
@@ -1842,7 +1858,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>43</v>
@@ -1860,7 +1876,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>44</v>
@@ -1878,7 +1894,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>45</v>
@@ -1896,7 +1912,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>46</v>
@@ -1914,7 +1930,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>47</v>
@@ -1932,7 +1948,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>49</v>
@@ -1947,18 +1963,18 @@
         <v>50</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>51</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>57</v>
@@ -1971,7 +1987,7 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>58</v>
@@ -1980,20 +1996,20 @@
     </row>
     <row r="49" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D49" s="2">
         <v>1</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>58</v>
@@ -2002,51 +2018,51 @@
     </row>
     <row r="50" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D50" s="2">
         <v>5</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>59</v>
@@ -2066,7 +2082,7 @@
     </row>
     <row r="53" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>65</v>
@@ -2086,81 +2102,81 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D54" s="2">
         <v>2</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="D55" s="2">
         <v>1</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="3" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56" s="2">
-        <v>1</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D57" s="2">
         <v>14</v>
@@ -2174,13 +2190,13 @@
     </row>
     <row r="58" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D58" s="2">
         <v>1</v>
@@ -2194,13 +2210,13 @@
     </row>
     <row r="59" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D59" s="2">
         <v>4</v>
@@ -2214,13 +2230,13 @@
     </row>
     <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="D60" s="2">
         <v>6</v>
@@ -2228,19 +2244,19 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="D61" s="2">
         <v>12</v>
@@ -2254,13 +2270,13 @@
     </row>
     <row r="62" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D62" s="2">
         <v>9</v>
@@ -2268,19 +2284,19 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D63" s="2">
         <v>7</v>
@@ -2288,7 +2304,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H63" s="2"/>
     </row>
@@ -2304,7 +2320,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>55</v>
@@ -2322,29 +2338,29 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>52</v>
@@ -2366,7 +2382,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>55</v>
@@ -2376,11 +2392,11 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H68" s="2"/>
     </row>
@@ -2396,29 +2412,29 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="D70" s="2">
         <v>1</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>68</v>
@@ -2440,7 +2456,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>72</v>
@@ -2460,7 +2476,7 @@
     </row>
     <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>75</v>
@@ -2480,167 +2496,173 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
       <c r="D74" s="2">
         <v>2</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F74" s="3"/>
-      <c r="G74" s="2"/>
+      <c r="G74" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="H74" s="2"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="D75" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F75" s="3"/>
-      <c r="G75" s="2"/>
+      <c r="G75" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D76" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F76" s="3"/>
-      <c r="G76" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C77" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D77" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F77" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="F77" s="3"/>
       <c r="G77" s="3" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>152</v>
+        <v>97</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="F78" s="2"/>
       <c r="G78" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="A79" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1</v>
+      </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
+      <c r="G79" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C81" s="4" t="s">
+      <c r="C82" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H81" s="2"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
@@ -2648,37 +2670,39 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="3" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="H82" s="2"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
+      <c r="G83" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="H83" s="2"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
@@ -2690,24 +2714,42 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
-      <c r="E85" s="3" t="s">
-        <v>143</v>
-      </c>
+      <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="3" t="s">
-        <v>143</v>
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2726,44 +2768,47 @@
     <hyperlink ref="E72" r:id="rId11"/>
     <hyperlink ref="G73" r:id="rId12"/>
     <hyperlink ref="E74" r:id="rId13"/>
-    <hyperlink ref="E75" r:id="rId14"/>
-    <hyperlink ref="E76" r:id="rId15"/>
-    <hyperlink ref="G76" r:id="rId16"/>
-    <hyperlink ref="H54" r:id="rId17"/>
-    <hyperlink ref="E55" r:id="rId18"/>
-    <hyperlink ref="G55" r:id="rId19"/>
-    <hyperlink ref="G56" r:id="rId20"/>
-    <hyperlink ref="E56" r:id="rId21"/>
-    <hyperlink ref="E77" r:id="rId22"/>
-    <hyperlink ref="G77" r:id="rId23"/>
-    <hyperlink ref="G78" r:id="rId24"/>
-    <hyperlink ref="G57" r:id="rId25"/>
-    <hyperlink ref="G58" r:id="rId26"/>
-    <hyperlink ref="G60" r:id="rId27" display="wilco"/>
-    <hyperlink ref="G61" r:id="rId28"/>
-    <hyperlink ref="G62" r:id="rId29" display="wilco"/>
-    <hyperlink ref="G63" r:id="rId30" display="wilco"/>
-    <hyperlink ref="G50" r:id="rId31"/>
-    <hyperlink ref="G59" r:id="rId32"/>
-    <hyperlink ref="G49" r:id="rId33"/>
-    <hyperlink ref="G81" r:id="rId34"/>
-    <hyperlink ref="G82" r:id="rId35"/>
-    <hyperlink ref="E85" r:id="rId36"/>
-    <hyperlink ref="H85" r:id="rId37"/>
-    <hyperlink ref="E54" r:id="rId38"/>
-    <hyperlink ref="H47" r:id="rId39"/>
-    <hyperlink ref="F47" r:id="rId40"/>
-    <hyperlink ref="G66" r:id="rId41"/>
-    <hyperlink ref="F66" r:id="rId42"/>
-    <hyperlink ref="G54" r:id="rId43"/>
-    <hyperlink ref="F50" r:id="rId44" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
-    <hyperlink ref="F49" r:id="rId45" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
-    <hyperlink ref="F48" r:id="rId46" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
-    <hyperlink ref="G51" r:id="rId47"/>
-    <hyperlink ref="E51" r:id="rId48"/>
+    <hyperlink ref="E77" r:id="rId14"/>
+    <hyperlink ref="G77" r:id="rId15"/>
+    <hyperlink ref="H54" r:id="rId16"/>
+    <hyperlink ref="E55" r:id="rId17"/>
+    <hyperlink ref="G55" r:id="rId18"/>
+    <hyperlink ref="G56" r:id="rId19"/>
+    <hyperlink ref="E56" r:id="rId20"/>
+    <hyperlink ref="E78" r:id="rId21"/>
+    <hyperlink ref="G78" r:id="rId22"/>
+    <hyperlink ref="G79" r:id="rId23"/>
+    <hyperlink ref="G57" r:id="rId24"/>
+    <hyperlink ref="G58" r:id="rId25"/>
+    <hyperlink ref="G60" r:id="rId26" display="wilco"/>
+    <hyperlink ref="G61" r:id="rId27"/>
+    <hyperlink ref="G62" r:id="rId28" display="wilco"/>
+    <hyperlink ref="G63" r:id="rId29" display="wilco"/>
+    <hyperlink ref="G50" r:id="rId30"/>
+    <hyperlink ref="G59" r:id="rId31"/>
+    <hyperlink ref="G49" r:id="rId32"/>
+    <hyperlink ref="G82" r:id="rId33"/>
+    <hyperlink ref="G83" r:id="rId34"/>
+    <hyperlink ref="E86" r:id="rId35"/>
+    <hyperlink ref="H86" r:id="rId36"/>
+    <hyperlink ref="E54" r:id="rId37"/>
+    <hyperlink ref="H47" r:id="rId38"/>
+    <hyperlink ref="F47" r:id="rId39"/>
+    <hyperlink ref="G66" r:id="rId40"/>
+    <hyperlink ref="F66" r:id="rId41"/>
+    <hyperlink ref="G54" r:id="rId42"/>
+    <hyperlink ref="F50" r:id="rId43" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
+    <hyperlink ref="F49" r:id="rId44" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
+    <hyperlink ref="F48" r:id="rId45" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
+    <hyperlink ref="G51" r:id="rId46"/>
+    <hyperlink ref="E51" r:id="rId47"/>
+    <hyperlink ref="G74" r:id="rId48"/>
+    <hyperlink ref="E75" r:id="rId49"/>
+    <hyperlink ref="G75" r:id="rId50"/>
+    <hyperlink ref="E76" r:id="rId51"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId49"/>
+  <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId52"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add vercro band for sensor unit to BOM list
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="193">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -350,10 +350,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SensorBoard_V1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>HbSensorBoard01</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -773,6 +769,22 @@
   </si>
   <si>
     <t>Lead Wire Cable 50mm</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SensorUnit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SensorUnit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Amazon</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1221,8 +1233,8 @@
   <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1279,7 @@
         <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
@@ -1283,7 +1295,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
@@ -1299,7 +1311,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -1315,7 +1327,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>16</v>
@@ -1331,7 +1343,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
@@ -1347,7 +1359,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
@@ -1363,7 +1375,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -1379,7 +1391,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1395,7 +1407,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1411,7 +1423,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -1427,7 +1439,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
@@ -1443,7 +1455,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>16</v>
@@ -1459,7 +1471,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
@@ -1475,7 +1487,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -1491,7 +1503,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -1507,7 +1519,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
@@ -1522,10 +1534,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
@@ -1541,7 +1553,7 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
@@ -1557,7 +1569,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>16</v>
@@ -1573,7 +1585,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -1589,7 +1601,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>16</v>
@@ -1605,7 +1617,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>16</v>
@@ -1621,7 +1633,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>16</v>
@@ -1637,7 +1649,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>16</v>
@@ -1653,7 +1665,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
@@ -1669,7 +1681,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>16</v>
@@ -1684,10 +1696,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>16</v>
@@ -1703,7 +1715,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>16</v>
@@ -1719,7 +1731,7 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>16</v>
@@ -1735,7 +1747,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>16</v>
@@ -1751,7 +1763,7 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>16</v>
@@ -1767,7 +1779,7 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>16</v>
@@ -1783,7 +1795,7 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>16</v>
@@ -1798,10 +1810,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>16</v>
@@ -1815,7 +1827,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>16</v>
@@ -1829,7 +1841,7 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>16</v>
@@ -1843,7 +1855,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>16</v>
@@ -1857,7 +1869,7 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>16</v>
@@ -1871,7 +1883,7 @@
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>16</v>
@@ -1885,7 +1897,7 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>16</v>
@@ -1898,7 +1910,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>3</v>
@@ -1980,10 +1992,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>16</v>
@@ -1998,10 +2010,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>16</v>
@@ -2017,7 +2029,7 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>16</v>
@@ -2033,7 +2045,7 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>16</v>
@@ -2049,7 +2061,7 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>16</v>
@@ -2065,7 +2077,7 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>16</v>
@@ -2081,7 +2093,7 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>16</v>
@@ -2096,10 +2108,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>16</v>
@@ -2115,7 +2127,7 @@
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>16</v>
@@ -2131,7 +2143,7 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>16</v>
@@ -2147,7 +2159,7 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>16</v>
@@ -2187,13 +2199,13 @@
         <v>10</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
@@ -2201,7 +2213,7 @@
         <v>71</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>18</v>
@@ -2211,10 +2223,10 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H60" s="2"/>
     </row>
@@ -2223,7 +2235,7 @@
         <v>71</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>69</v>
@@ -2233,7 +2245,7 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>14</v>
@@ -2255,7 +2267,7 @@
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>65</v>
@@ -2267,7 +2279,7 @@
         <v>71</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>62</v>
@@ -2276,11 +2288,11 @@
         <v>2</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H63" s="2"/>
     </row>
@@ -2329,7 +2341,7 @@
         <v>71</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>41</v>
@@ -2338,16 +2350,16 @@
         <v>2</v>
       </c>
       <c r="E66" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="H66" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -2367,10 +2379,10 @@
         <v>36</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H67" s="2"/>
     </row>
@@ -2388,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="3" t="s">
@@ -2401,10 +2413,10 @@
         <v>71</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D69" s="2">
         <v>37</v>
@@ -2421,10 +2433,10 @@
         <v>71</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="D70" s="2">
         <v>4</v>
@@ -2450,7 +2462,7 @@
         <v>6</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="3" t="s">
@@ -2492,7 +2504,7 @@
         <v>9</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="3" t="s">
@@ -2514,7 +2526,7 @@
         <v>7</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="3" t="s">
@@ -2555,7 +2567,7 @@
         <v>73</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>72</v>
@@ -2565,7 +2577,7 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>38</v>
@@ -2577,20 +2589,20 @@
         <v>73</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="D78" s="2">
         <v>2</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H78" s="2"/>
     </row>
@@ -2606,11 +2618,11 @@
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H79" s="2"/>
     </row>
@@ -2638,11 +2650,11 @@
         <v>1</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H81" s="2"/>
     </row>
@@ -2654,13 +2666,13 @@
         <v>23</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3" t="s">
@@ -2716,7 +2728,7 @@
         <v>31</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
@@ -2726,7 +2738,7 @@
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H85" s="2"/>
     </row>
@@ -2735,7 +2747,7 @@
         <v>74</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>35</v>
@@ -2755,10 +2767,10 @@
         <v>74</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
@@ -2780,7 +2792,7 @@
         <v>46</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D88" s="2">
         <v>4</v>
@@ -2802,7 +2814,7 @@
         <v>49</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
@@ -2820,7 +2832,7 @@
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D90" s="2">
         <v>2</v>
@@ -2836,7 +2848,7 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D91" s="2">
         <v>2</v>
@@ -2858,138 +2870,151 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D93" s="2">
         <v>1</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H93" s="2"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="D94" s="2">
-        <v>1</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H94" s="2"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D95" s="2">
-        <v>1</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H96" s="2"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="D97" s="2">
         <v>1</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H97" s="2"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="2"/>
+      <c r="A99" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F99" s="2"/>
+      <c r="G99" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H99" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3062,9 +3087,11 @@
     <hyperlink ref="E73" r:id="rId57"/>
     <hyperlink ref="E74" r:id="rId58" display="Hirosugi-Keiki(SRU-2010)"/>
     <hyperlink ref="F67" r:id="rId59" display="https://www.pololu.com/product/1058"/>
+    <hyperlink ref="G99" r:id="rId60"/>
+    <hyperlink ref="E99" r:id="rId61" display="Amaaon"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId60"/>
+  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId62"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
correct some mistakes in BOM
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$101</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$100</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="198">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -395,17 +395,6 @@
   </si>
   <si>
     <t>mouser</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>flatScrewM2L6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Flat screw
--Shaft diameter:2
--Head diameter:4
--Length:6</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1258,11 +1247,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1296,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
@@ -1323,7 +1312,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
@@ -1339,7 +1328,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -1355,7 +1344,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1371,7 +1360,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1387,7 +1376,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -1403,7 +1392,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
@@ -1419,7 +1408,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1435,7 +1424,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
@@ -1451,7 +1440,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -1467,7 +1456,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>15</v>
@@ -1483,7 +1472,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>15</v>
@@ -1499,7 +1488,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
@@ -1515,7 +1504,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
@@ -1531,7 +1520,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>15</v>
@@ -1547,7 +1536,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>15</v>
@@ -1562,10 +1551,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>15</v>
@@ -1581,7 +1570,7 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
@@ -1597,7 +1586,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
@@ -1613,7 +1602,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>15</v>
@@ -1629,7 +1618,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>15</v>
@@ -1645,7 +1634,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>15</v>
@@ -1661,7 +1650,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
@@ -1677,7 +1666,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>15</v>
@@ -1693,7 +1682,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>15</v>
@@ -1709,7 +1698,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>15</v>
@@ -1724,10 +1713,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>15</v>
@@ -1743,7 +1732,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>15</v>
@@ -1759,7 +1748,7 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>15</v>
@@ -1775,7 +1764,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>15</v>
@@ -1791,7 +1780,7 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>15</v>
@@ -1807,7 +1796,7 @@
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>15</v>
@@ -1823,7 +1812,7 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>15</v>
@@ -1838,10 +1827,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>15</v>
@@ -1855,7 +1844,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>15</v>
@@ -1869,7 +1858,7 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>15</v>
@@ -1883,7 +1872,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>15</v>
@@ -1897,7 +1886,7 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>15</v>
@@ -1911,7 +1900,7 @@
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>15</v>
@@ -1925,7 +1914,7 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>15</v>
@@ -1938,7 +1927,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>3</v>
@@ -2020,10 +2009,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>15</v>
@@ -2038,10 +2027,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>15</v>
@@ -2057,7 +2046,7 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>15</v>
@@ -2073,7 +2062,7 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>15</v>
@@ -2089,7 +2078,7 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>15</v>
@@ -2105,7 +2094,7 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>15</v>
@@ -2121,7 +2110,7 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>15</v>
@@ -2136,10 +2125,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>15</v>
@@ -2155,7 +2144,7 @@
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>15</v>
@@ -2171,7 +2160,7 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>15</v>
@@ -2187,7 +2176,7 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>15</v>
@@ -2241,7 +2230,7 @@
         <v>69</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>17</v>
@@ -2251,10 +2240,10 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H60" s="2"/>
     </row>
@@ -2263,7 +2252,7 @@
         <v>69</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>67</v>
@@ -2273,7 +2262,7 @@
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>14</v>
@@ -2295,7 +2284,7 @@
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>63</v>
@@ -2307,7 +2296,7 @@
         <v>69</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>60</v>
@@ -2316,11 +2305,11 @@
         <v>2</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H63" s="2"/>
     </row>
@@ -2329,13 +2318,13 @@
         <v>69</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D64" s="2">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -2369,7 +2358,7 @@
         <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>39</v>
@@ -2378,16 +2367,16 @@
         <v>2</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
@@ -2407,10 +2396,10 @@
         <v>34</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H67" s="2"/>
     </row>
@@ -2419,20 +2408,20 @@
         <v>69</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>198</v>
       </c>
       <c r="D68" s="2">
         <v>2</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H68" s="2"/>
     </row>
@@ -2441,20 +2430,20 @@
         <v>69</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H69" s="2"/>
     </row>
@@ -2472,7 +2461,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="3" t="s">
@@ -2505,18 +2494,20 @@
         <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D72" s="2">
-        <v>4</v>
-      </c>
-      <c r="E72" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="F72" s="2"/>
       <c r="G72" s="3" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="H72" s="2"/>
     </row>
@@ -2525,40 +2516,40 @@
         <v>69</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D73" s="2">
-        <v>6</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>157</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="3" t="s">
-        <v>51</v>
+        <v>191</v>
       </c>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>50</v>
+      <c r="B74" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D74" s="2">
-        <v>5</v>
-      </c>
-      <c r="E74" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="F74" s="2"/>
       <c r="G74" s="3" t="s">
-        <v>193</v>
+        <v>56</v>
       </c>
       <c r="H74" s="2"/>
     </row>
@@ -2567,50 +2558,46 @@
         <v>69</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D75" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D76" s="2">
-        <v>7</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>182</v>
-      </c>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="A77" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -2621,17 +2608,21 @@
         <v>71</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>13</v>
+        <v>158</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
+      <c r="F78" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2639,20 +2630,20 @@
         <v>71</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>70</v>
+        <v>163</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="D79" s="2">
-        <v>1</v>
-      </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="3" t="s">
-        <v>86</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F79" s="3"/>
       <c r="G79" s="3" t="s">
-        <v>36</v>
+        <v>165</v>
       </c>
       <c r="H79" s="2"/>
     </row>
@@ -2661,134 +2652,134 @@
         <v>71</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D80" s="2">
-        <v>2</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3" t="s">
-        <v>167</v>
+        <v>13</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="H80" s="2"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
       <c r="D81" s="2"/>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2" t="s">
+      <c r="F82" s="2"/>
+      <c r="G82" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H81" s="2"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
-      <c r="E83" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2" t="s">
-        <v>81</v>
+      <c r="E83" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C84" s="2"/>
       <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C85" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
-      <c r="E85" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="D86" s="2">
         <v>1</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="H86" s="2"/>
     </row>
@@ -2797,21 +2788,19 @@
         <v>72</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="D87" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F87" s="3"/>
-      <c r="G87" s="3" t="s">
-        <v>179</v>
-      </c>
+      <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2819,19 +2808,21 @@
         <v>72</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D88" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F88" s="3"/>
-      <c r="G88" s="2"/>
+      <c r="G88" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="H88" s="2"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -2839,20 +2830,20 @@
         <v>72</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>96</v>
+        <v>44</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D89" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F89" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="F89" s="2"/>
       <c r="G89" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H89" s="2"/>
     </row>
@@ -2861,20 +2852,18 @@
         <v>72</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>97</v>
+        <v>47</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="D90" s="2">
-        <v>4</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H90" s="2"/>
     </row>
@@ -2882,20 +2871,16 @@
       <c r="A91" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B91" s="2"/>
       <c r="C91" s="4" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="D91" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="G91" s="3"/>
       <c r="H91" s="2"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2904,7 +2889,7 @@
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D92" s="2">
         <v>2</v>
@@ -2915,182 +2900,166 @@
       <c r="H92" s="2"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="A93" s="2"/>
       <c r="B93" s="2"/>
-      <c r="C93" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D93" s="2">
-        <v>2</v>
-      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
-      <c r="G93" s="3"/>
+      <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
+      <c r="A94" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
+      <c r="G94" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="H94" s="2"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>74</v>
+        <v>168</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="D95" s="2">
         <v>1</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>82</v>
+      <c r="E95" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="F95" s="2"/>
-      <c r="G95" s="2" t="s">
-        <v>82</v>
+      <c r="G95" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H96" s="2"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>75</v>
+        <v>174</v>
       </c>
       <c r="D97" s="2">
         <v>1</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H97" s="2"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="D98" s="2">
         <v>1</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H98" s="2"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>174</v>
+        <v>77</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
       <c r="D99" s="2">
         <v>1</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="F99" s="2"/>
-      <c r="G99" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F100" s="2"/>
+      <c r="G100" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D100" s="2">
-        <v>1</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D101" s="2"/>
-      <c r="E101" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F101" s="2"/>
-      <c r="G101" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H101" s="2"/>
+      <c r="H100" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3106,72 +3075,71 @@
   <hyperlinks>
     <hyperlink ref="E59" r:id="rId1"/>
     <hyperlink ref="G59" r:id="rId2"/>
-    <hyperlink ref="G80" r:id="rId3"/>
-    <hyperlink ref="E80" r:id="rId4"/>
+    <hyperlink ref="G79" r:id="rId3"/>
+    <hyperlink ref="E79" r:id="rId4"/>
     <hyperlink ref="G60" r:id="rId5" location="prettyphoto/0/"/>
     <hyperlink ref="G64" r:id="rId6"/>
     <hyperlink ref="G65" r:id="rId7"/>
-    <hyperlink ref="G84" r:id="rId8"/>
-    <hyperlink ref="E84" r:id="rId9" display="SeedStudio"/>
-    <hyperlink ref="G85" r:id="rId10"/>
-    <hyperlink ref="E85" r:id="rId11"/>
-    <hyperlink ref="G86" r:id="rId12"/>
-    <hyperlink ref="E87" r:id="rId13"/>
-    <hyperlink ref="E89" r:id="rId14"/>
-    <hyperlink ref="G89" r:id="rId15"/>
+    <hyperlink ref="G83" r:id="rId8"/>
+    <hyperlink ref="E83" r:id="rId9" display="SeedStudio"/>
+    <hyperlink ref="G84" r:id="rId10"/>
+    <hyperlink ref="E84" r:id="rId11"/>
+    <hyperlink ref="G85" r:id="rId12"/>
+    <hyperlink ref="E86" r:id="rId13"/>
+    <hyperlink ref="E88" r:id="rId14"/>
+    <hyperlink ref="G88" r:id="rId15"/>
     <hyperlink ref="E67" r:id="rId16"/>
     <hyperlink ref="G67" r:id="rId17"/>
     <hyperlink ref="G70" r:id="rId18"/>
     <hyperlink ref="E70" r:id="rId19"/>
-    <hyperlink ref="E90" r:id="rId20"/>
-    <hyperlink ref="G90" r:id="rId21"/>
-    <hyperlink ref="G91" r:id="rId22"/>
+    <hyperlink ref="E89" r:id="rId20"/>
+    <hyperlink ref="G89" r:id="rId21"/>
+    <hyperlink ref="G90" r:id="rId22"/>
     <hyperlink ref="G71" r:id="rId23"/>
-    <hyperlink ref="G73" r:id="rId24" display="wilco"/>
-    <hyperlink ref="G74" r:id="rId25"/>
-    <hyperlink ref="G75" r:id="rId26" display="wilco"/>
-    <hyperlink ref="G76" r:id="rId27" display="wilco"/>
+    <hyperlink ref="G72" r:id="rId24" display="wilco"/>
+    <hyperlink ref="G73" r:id="rId25"/>
+    <hyperlink ref="G74" r:id="rId26" display="wilco"/>
+    <hyperlink ref="G75" r:id="rId27" display="wilco"/>
     <hyperlink ref="G62" r:id="rId28" location="prettyphoto/83/"/>
-    <hyperlink ref="G72" r:id="rId29"/>
-    <hyperlink ref="G61" r:id="rId30"/>
-    <hyperlink ref="G97" r:id="rId31"/>
-    <hyperlink ref="E100" r:id="rId32"/>
-    <hyperlink ref="H100" r:id="rId33"/>
-    <hyperlink ref="H59" r:id="rId34"/>
-    <hyperlink ref="F59" r:id="rId35"/>
-    <hyperlink ref="G79" r:id="rId36"/>
-    <hyperlink ref="F79" r:id="rId37"/>
-    <hyperlink ref="G66" r:id="rId38" display="Amazon.jp"/>
-    <hyperlink ref="F62" r:id="rId39" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
-    <hyperlink ref="F61" r:id="rId40" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
-    <hyperlink ref="F60" r:id="rId41" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
-    <hyperlink ref="G63" r:id="rId42"/>
-    <hyperlink ref="E63" r:id="rId43"/>
-    <hyperlink ref="G87" r:id="rId44"/>
-    <hyperlink ref="E88" r:id="rId45"/>
-    <hyperlink ref="E73" r:id="rId46"/>
-    <hyperlink ref="E66" r:id="rId47"/>
-    <hyperlink ref="F66" r:id="rId48"/>
-    <hyperlink ref="H66" r:id="rId49"/>
-    <hyperlink ref="E96" r:id="rId50"/>
-    <hyperlink ref="G96" r:id="rId51"/>
+    <hyperlink ref="G61" r:id="rId29"/>
+    <hyperlink ref="G96" r:id="rId30"/>
+    <hyperlink ref="E99" r:id="rId31"/>
+    <hyperlink ref="H99" r:id="rId32"/>
+    <hyperlink ref="H59" r:id="rId33"/>
+    <hyperlink ref="F59" r:id="rId34"/>
+    <hyperlink ref="G78" r:id="rId35"/>
+    <hyperlink ref="F78" r:id="rId36"/>
+    <hyperlink ref="G66" r:id="rId37" display="Amazon.jp"/>
+    <hyperlink ref="F62" r:id="rId38" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
+    <hyperlink ref="F61" r:id="rId39" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
+    <hyperlink ref="F60" r:id="rId40" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
+    <hyperlink ref="G63" r:id="rId41"/>
+    <hyperlink ref="E63" r:id="rId42"/>
+    <hyperlink ref="G86" r:id="rId43"/>
+    <hyperlink ref="E87" r:id="rId44"/>
+    <hyperlink ref="E72" r:id="rId45"/>
+    <hyperlink ref="E66" r:id="rId46"/>
+    <hyperlink ref="F66" r:id="rId47"/>
+    <hyperlink ref="H66" r:id="rId48"/>
+    <hyperlink ref="E95" r:id="rId49"/>
+    <hyperlink ref="G95" r:id="rId50"/>
+    <hyperlink ref="E97" r:id="rId51"/>
     <hyperlink ref="E98" r:id="rId52"/>
-    <hyperlink ref="E99" r:id="rId53"/>
+    <hyperlink ref="G97" r:id="rId53"/>
     <hyperlink ref="G98" r:id="rId54"/>
-    <hyperlink ref="G99" r:id="rId55"/>
-    <hyperlink ref="E97" r:id="rId56"/>
-    <hyperlink ref="E75" r:id="rId57"/>
-    <hyperlink ref="E76" r:id="rId58" display="Hirosugi-Keiki(SRU-2010)"/>
-    <hyperlink ref="F67" r:id="rId59" display="https://www.pololu.com/product/1058"/>
-    <hyperlink ref="G101" r:id="rId60"/>
-    <hyperlink ref="E101" r:id="rId61" display="Amaaon"/>
-    <hyperlink ref="G68" r:id="rId62"/>
-    <hyperlink ref="G69" r:id="rId63"/>
-    <hyperlink ref="E68" r:id="rId64"/>
-    <hyperlink ref="E69" r:id="rId65"/>
+    <hyperlink ref="E96" r:id="rId55"/>
+    <hyperlink ref="E74" r:id="rId56"/>
+    <hyperlink ref="E75" r:id="rId57" display="Hirosugi-Keiki(SRU-2010)"/>
+    <hyperlink ref="F67" r:id="rId58" display="https://www.pololu.com/product/1058"/>
+    <hyperlink ref="G100" r:id="rId59"/>
+    <hyperlink ref="E100" r:id="rId60" display="Amaaon"/>
+    <hyperlink ref="G68" r:id="rId61"/>
+    <hyperlink ref="G69" r:id="rId62"/>
+    <hyperlink ref="E68" r:id="rId63"/>
+    <hyperlink ref="E69" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId66"/>
+  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId65"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
correct the number of screw
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -1250,8 +1250,8 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2324,7 @@
         <v>190</v>
       </c>
       <c r="D64" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>

</xml_diff>

<commit_message>
divided MainFrameA into two pieces.
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$100</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$101</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="199">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -802,6 +802,10 @@
   </si>
   <si>
     <t>Mouser</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sensor Cushion</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -915,7 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -945,6 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -1247,11 +1252,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3051,7 +3056,9 @@
       <c r="C100" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D100" s="2"/>
+      <c r="D100" s="2">
+        <v>1</v>
+      </c>
       <c r="E100" s="3" t="s">
         <v>188</v>
       </c>
@@ -3060,6 +3067,20 @@
         <v>187</v>
       </c>
       <c r="H100" s="2"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D101" s="13">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
change the number of screw in BOM
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$101</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$100</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="200">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -806,6 +806,10 @@
   </si>
   <si>
     <t>Sensor Cushion</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NA</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -931,6 +935,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,7 +954,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -1252,11 +1256,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H101"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1301,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1315,7 +1319,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>99</v>
       </c>
@@ -1331,7 +1335,7 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>100</v>
       </c>
@@ -1347,7 +1351,7 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>101</v>
       </c>
@@ -1363,7 +1367,7 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>102</v>
       </c>
@@ -1379,7 +1383,7 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>103</v>
       </c>
@@ -1395,7 +1399,7 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>104</v>
       </c>
@@ -1411,7 +1415,7 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>105</v>
       </c>
@@ -1427,7 +1431,7 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>106</v>
       </c>
@@ -1443,7 +1447,7 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
         <v>107</v>
       </c>
@@ -1459,7 +1463,7 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>108</v>
       </c>
@@ -1475,7 +1479,7 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
         <v>109</v>
       </c>
@@ -1491,7 +1495,7 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="2" t="s">
         <v>110</v>
       </c>
@@ -1507,7 +1511,7 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>111</v>
       </c>
@@ -1523,7 +1527,7 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
         <v>112</v>
       </c>
@@ -1539,7 +1543,7 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>113</v>
       </c>
@@ -1555,7 +1559,7 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>124</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1573,7 +1577,7 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
         <v>115</v>
       </c>
@@ -1589,7 +1593,7 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>116</v>
       </c>
@@ -1605,7 +1609,7 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="2" t="s">
         <v>117</v>
       </c>
@@ -1621,7 +1625,7 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="2" t="s">
         <v>118</v>
       </c>
@@ -1637,7 +1641,7 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="2" t="s">
         <v>119</v>
       </c>
@@ -1653,7 +1657,7 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
         <v>120</v>
       </c>
@@ -1669,7 +1673,7 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
         <v>121</v>
       </c>
@@ -1685,7 +1689,7 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>122</v>
       </c>
@@ -1701,7 +1705,7 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
         <v>123</v>
       </c>
@@ -1717,7 +1721,7 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>131</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1735,7 +1739,7 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="2" t="s">
         <v>126</v>
       </c>
@@ -1751,7 +1755,7 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
         <v>127</v>
       </c>
@@ -1767,7 +1771,7 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
         <v>128</v>
       </c>
@@ -1783,7 +1787,7 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
         <v>121</v>
       </c>
@@ -1799,7 +1803,7 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="2" t="s">
         <v>129</v>
       </c>
@@ -1815,7 +1819,7 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="2" t="s">
         <v>130</v>
       </c>
@@ -1831,7 +1835,7 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
         <v>154</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1847,7 +1851,7 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="2" t="s">
         <v>148</v>
       </c>
@@ -1861,7 +1865,7 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="2" t="s">
         <v>149</v>
       </c>
@@ -1875,7 +1879,7 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="2" t="s">
         <v>150</v>
       </c>
@@ -1889,7 +1893,7 @@
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="2" t="s">
         <v>151</v>
       </c>
@@ -1903,7 +1907,7 @@
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="2" t="s">
         <v>152</v>
       </c>
@@ -1917,7 +1921,7 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="2" t="s">
         <v>153</v>
       </c>
@@ -1931,7 +1935,7 @@
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="11" t="s">
         <v>132</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1949,7 +1953,7 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
@@ -1965,7 +1969,7 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="2" t="s">
         <v>5</v>
       </c>
@@ -1981,7 +1985,7 @@
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="2" t="s">
         <v>6</v>
       </c>
@@ -1997,7 +2001,7 @@
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="2" t="s">
         <v>7</v>
       </c>
@@ -2031,7 +2035,7 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="8" t="s">
         <v>141</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2049,7 +2053,7 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
+      <c r="A49" s="9"/>
       <c r="B49" s="2" t="s">
         <v>136</v>
       </c>
@@ -2065,7 +2069,7 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
+      <c r="A50" s="9"/>
       <c r="B50" s="2" t="s">
         <v>137</v>
       </c>
@@ -2081,7 +2085,7 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+      <c r="A51" s="9"/>
       <c r="B51" s="2" t="s">
         <v>138</v>
       </c>
@@ -2097,7 +2101,7 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
+      <c r="A52" s="9"/>
       <c r="B52" s="2" t="s">
         <v>139</v>
       </c>
@@ -2113,7 +2117,7 @@
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="2" t="s">
         <v>140</v>
       </c>
@@ -2129,7 +2133,7 @@
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="8" t="s">
         <v>146</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -2147,7 +2151,7 @@
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="2" t="s">
         <v>143</v>
       </c>
@@ -2163,7 +2167,7 @@
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
+      <c r="A56" s="9"/>
       <c r="B56" s="2" t="s">
         <v>144</v>
       </c>
@@ -2179,7 +2183,7 @@
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="9"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="2" t="s">
         <v>145</v>
       </c>
@@ -2485,7 +2489,7 @@
         <v>84</v>
       </c>
       <c r="D71" s="2">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -2603,9 +2607,13 @@
       <c r="D77" s="2">
         <v>1</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
+      <c r="G77" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="H77" s="2"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -2653,116 +2661,118 @@
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
       <c r="D80" s="2"/>
-      <c r="E80" s="2" t="s">
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2" t="s">
+      <c r="F81" s="2"/>
+      <c r="G81" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2" t="s">
-        <v>81</v>
+      <c r="E82" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C83" s="2"/>
       <c r="D83" s="2">
         <v>1</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C84" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
       </c>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="H85" s="2"/>
     </row>
@@ -2771,21 +2781,19 @@
         <v>72</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="D86" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F86" s="3"/>
-      <c r="G86" s="3" t="s">
-        <v>177</v>
-      </c>
+      <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -2793,19 +2801,21 @@
         <v>72</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D87" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F87" s="3"/>
-      <c r="G87" s="2"/>
+      <c r="G87" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2813,20 +2823,20 @@
         <v>72</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>94</v>
+        <v>44</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D88" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F88" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="F88" s="2"/>
       <c r="G88" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H88" s="2"/>
     </row>
@@ -2835,20 +2845,18 @@
         <v>72</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>95</v>
+        <v>47</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="D89" s="2">
-        <v>4</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H89" s="2"/>
     </row>
@@ -2856,20 +2864,16 @@
       <c r="A90" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B90" s="2"/>
       <c r="C90" s="4" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="D90" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
-      <c r="G90" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="G90" s="3"/>
       <c r="H90" s="2"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -2878,7 +2882,7 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D91" s="2">
         <v>2</v>
@@ -2889,29 +2893,35 @@
       <c r="H91" s="2"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="A92" s="2"/>
       <c r="B92" s="2"/>
-      <c r="C92" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D92" s="2">
-        <v>2</v>
-      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
-      <c r="G92" s="3"/>
+      <c r="G92" s="2"/>
       <c r="H92" s="2"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
+      <c r="A93" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
+      <c r="G93" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="H93" s="2"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -2919,20 +2929,20 @@
         <v>185</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>74</v>
+        <v>168</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="D94" s="2">
         <v>1</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>82</v>
+      <c r="E94" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="F94" s="2"/>
-      <c r="G94" s="2" t="s">
-        <v>82</v>
+      <c r="G94" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="H94" s="2"/>
     </row>
@@ -2941,20 +2951,20 @@
         <v>185</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D95" s="2">
         <v>1</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H95" s="2"/>
     </row>
@@ -2963,20 +2973,20 @@
         <v>185</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>75</v>
+        <v>174</v>
       </c>
       <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H96" s="2"/>
     </row>
@@ -2985,10 +2995,10 @@
         <v>185</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D97" s="2">
         <v>1</v>
@@ -3007,78 +3017,56 @@
         <v>185</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>172</v>
+        <v>77</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>173</v>
+        <v>76</v>
       </c>
       <c r="D98" s="2">
         <v>1</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="F98" s="2"/>
-      <c r="G98" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>77</v>
+        <v>193</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>76</v>
+        <v>193</v>
       </c>
       <c r="D99" s="2">
         <v>1</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="G99" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H99" s="2"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D100" s="2">
-        <v>1</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F100" s="2"/>
-      <c r="G100" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H100" s="2"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B100" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C100" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D101" s="13">
+      <c r="D100" s="7">
         <v>1</v>
       </c>
     </row>
@@ -3101,21 +3089,21 @@
     <hyperlink ref="G60" r:id="rId5" location="prettyphoto/0/"/>
     <hyperlink ref="G64" r:id="rId6"/>
     <hyperlink ref="G65" r:id="rId7"/>
-    <hyperlink ref="G83" r:id="rId8"/>
-    <hyperlink ref="E83" r:id="rId9" display="SeedStudio"/>
-    <hyperlink ref="G84" r:id="rId10"/>
-    <hyperlink ref="E84" r:id="rId11"/>
-    <hyperlink ref="G85" r:id="rId12"/>
-    <hyperlink ref="E86" r:id="rId13"/>
-    <hyperlink ref="E88" r:id="rId14"/>
-    <hyperlink ref="G88" r:id="rId15"/>
+    <hyperlink ref="G82" r:id="rId8"/>
+    <hyperlink ref="E82" r:id="rId9" display="SeedStudio"/>
+    <hyperlink ref="G83" r:id="rId10"/>
+    <hyperlink ref="E83" r:id="rId11"/>
+    <hyperlink ref="G84" r:id="rId12"/>
+    <hyperlink ref="E85" r:id="rId13"/>
+    <hyperlink ref="E87" r:id="rId14"/>
+    <hyperlink ref="G87" r:id="rId15"/>
     <hyperlink ref="E67" r:id="rId16"/>
     <hyperlink ref="G67" r:id="rId17"/>
     <hyperlink ref="G70" r:id="rId18"/>
     <hyperlink ref="E70" r:id="rId19"/>
-    <hyperlink ref="E89" r:id="rId20"/>
-    <hyperlink ref="G89" r:id="rId21"/>
-    <hyperlink ref="G90" r:id="rId22"/>
+    <hyperlink ref="E88" r:id="rId20"/>
+    <hyperlink ref="G88" r:id="rId21"/>
+    <hyperlink ref="G89" r:id="rId22"/>
     <hyperlink ref="G71" r:id="rId23"/>
     <hyperlink ref="G72" r:id="rId24" display="wilco"/>
     <hyperlink ref="G73" r:id="rId25"/>
@@ -3123,9 +3111,9 @@
     <hyperlink ref="G75" r:id="rId27" display="wilco"/>
     <hyperlink ref="G62" r:id="rId28" location="prettyphoto/83/"/>
     <hyperlink ref="G61" r:id="rId29"/>
-    <hyperlink ref="G96" r:id="rId30"/>
-    <hyperlink ref="E99" r:id="rId31"/>
-    <hyperlink ref="H99" r:id="rId32"/>
+    <hyperlink ref="G95" r:id="rId30"/>
+    <hyperlink ref="E98" r:id="rId31"/>
+    <hyperlink ref="H98" r:id="rId32"/>
     <hyperlink ref="H59" r:id="rId33"/>
     <hyperlink ref="F59" r:id="rId34"/>
     <hyperlink ref="G78" r:id="rId35"/>
@@ -3136,24 +3124,24 @@
     <hyperlink ref="F60" r:id="rId40" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
     <hyperlink ref="G63" r:id="rId41"/>
     <hyperlink ref="E63" r:id="rId42"/>
-    <hyperlink ref="G86" r:id="rId43"/>
-    <hyperlink ref="E87" r:id="rId44"/>
+    <hyperlink ref="G85" r:id="rId43"/>
+    <hyperlink ref="E86" r:id="rId44"/>
     <hyperlink ref="E72" r:id="rId45"/>
     <hyperlink ref="E66" r:id="rId46"/>
     <hyperlink ref="F66" r:id="rId47"/>
     <hyperlink ref="H66" r:id="rId48"/>
-    <hyperlink ref="E95" r:id="rId49"/>
-    <hyperlink ref="G95" r:id="rId50"/>
-    <hyperlink ref="E97" r:id="rId51"/>
-    <hyperlink ref="E98" r:id="rId52"/>
-    <hyperlink ref="G97" r:id="rId53"/>
-    <hyperlink ref="G98" r:id="rId54"/>
-    <hyperlink ref="E96" r:id="rId55"/>
+    <hyperlink ref="E94" r:id="rId49"/>
+    <hyperlink ref="G94" r:id="rId50"/>
+    <hyperlink ref="E96" r:id="rId51"/>
+    <hyperlink ref="E97" r:id="rId52"/>
+    <hyperlink ref="G96" r:id="rId53"/>
+    <hyperlink ref="G97" r:id="rId54"/>
+    <hyperlink ref="E95" r:id="rId55"/>
     <hyperlink ref="E74" r:id="rId56"/>
     <hyperlink ref="E75" r:id="rId57" display="Hirosugi-Keiki(SRU-2010)"/>
     <hyperlink ref="F67" r:id="rId58" display="https://www.pololu.com/product/1058"/>
-    <hyperlink ref="G100" r:id="rId59"/>
-    <hyperlink ref="E100" r:id="rId60" display="Amaaon"/>
+    <hyperlink ref="G99" r:id="rId59"/>
+    <hyperlink ref="E99" r:id="rId60" display="Amaaon"/>
     <hyperlink ref="G68" r:id="rId61"/>
     <hyperlink ref="G69" r:id="rId62"/>
     <hyperlink ref="E68" r:id="rId63"/>

</xml_diff>

<commit_message>
make assemble file for SLS printing
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$100</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$99</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="199">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>HbBackCover02.stl</t>
-  </si>
-  <si>
-    <t>HbButtonU01.stl</t>
   </si>
   <si>
     <t>HbFingerLockButton05.stl</t>
@@ -1256,11 +1253,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E103" sqref="E103"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1321,7 @@
         <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -1527,7 +1524,7 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>112</v>
       </c>
@@ -1543,7 +1540,9 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>113</v>
       </c>
@@ -1559,9 +1558,7 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>124</v>
-      </c>
+      <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
         <v>114</v>
       </c>
@@ -1689,7 +1686,7 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>122</v>
       </c>
@@ -1705,9 +1702,11 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>15</v>
@@ -1721,9 +1720,7 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>131</v>
-      </c>
+      <c r="A28" s="9"/>
       <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
@@ -1773,7 +1770,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>15</v>
@@ -1789,7 +1786,7 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>15</v>
@@ -1803,7 +1800,7 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="2" t="s">
         <v>129</v>
       </c>
@@ -1819,25 +1816,23 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="2">
-        <v>1</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>154</v>
-      </c>
+      <c r="A35" s="9"/>
       <c r="B35" s="2" t="s">
         <v>147</v>
       </c>
@@ -1921,25 +1916,27 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="A41" s="11" t="s">
+        <v>131</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>153</v>
+        <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="2">
+        <v>3</v>
+      </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>132</v>
-      </c>
+      <c r="A42" s="12"/>
       <c r="B42" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>15</v>
@@ -1955,7 +1952,7 @@
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>15</v>
@@ -1971,7 +1968,7 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>15</v>
@@ -1985,9 +1982,9 @@
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>15</v>
@@ -2001,15 +1998,17 @@
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+      <c r="A46" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="B46" s="2" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D46" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2017,11 +2016,11 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>15</v>
@@ -2035,9 +2034,7 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>141</v>
-      </c>
+      <c r="A48" s="9"/>
       <c r="B48" s="2" t="s">
         <v>135</v>
       </c>
@@ -2101,7 +2098,7 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="2" t="s">
         <v>139</v>
       </c>
@@ -2117,9 +2114,11 @@
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
+      <c r="A53" s="8" t="s">
+        <v>145</v>
+      </c>
       <c r="B53" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>15</v>
@@ -2133,9 +2132,7 @@
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
-        <v>146</v>
-      </c>
+      <c r="A54" s="9"/>
       <c r="B54" s="2" t="s">
         <v>142</v>
       </c>
@@ -2167,7 +2164,7 @@
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
+      <c r="A56" s="10"/>
       <c r="B56" s="2" t="s">
         <v>144</v>
       </c>
@@ -2183,142 +2180,146 @@
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="2">
-        <v>1</v>
-      </c>
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>8</v>
+        <v>158</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D59" s="2">
-        <v>1</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>80</v>
+        <v>6</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>159</v>
+      <c r="B60" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D60" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>157</v>
+      <c r="B61" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D62" s="2">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="5" t="s">
-        <v>90</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" s="2"/>
       <c r="G62" s="3" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>60</v>
+        <v>189</v>
       </c>
       <c r="D63" s="2">
-        <v>2</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>93</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="H63" s="2"/>
     </row>
@@ -2327,13 +2328,13 @@
         <v>69</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>189</v>
+        <v>19</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>190</v>
+        <v>20</v>
       </c>
       <c r="D64" s="2">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -2342,71 +2343,73 @@
       </c>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D65" s="2">
-        <v>6</v>
-      </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="G65" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D66" s="2">
-        <v>2</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>160</v>
+        <v>1</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>40</v>
+        <v>195</v>
       </c>
       <c r="D67" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>182</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="F67" s="5"/>
       <c r="G67" s="3" t="s">
         <v>96</v>
       </c>
@@ -2420,13 +2423,13 @@
         <v>194</v>
       </c>
       <c r="C68" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="D68" s="2">
-        <v>2</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="3" t="s">
@@ -2434,47 +2437,45 @@
       </c>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>196</v>
+        <v>42</v>
       </c>
       <c r="D69" s="2">
         <v>1</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>161</v>
+      </c>
+      <c r="F69" s="2"/>
       <c r="G69" s="3" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="D70" s="2">
-        <v>1</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>162</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="H70" s="2"/>
     </row>
@@ -2483,18 +2484,20 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D71" s="2">
-        <v>46</v>
-      </c>
-      <c r="E71" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="F71" s="2"/>
       <c r="G71" s="3" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="H71" s="2"/>
     </row>
@@ -2503,40 +2506,40 @@
         <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D72" s="2">
-        <v>6</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>155</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="3" t="s">
-        <v>51</v>
+        <v>190</v>
       </c>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>50</v>
+      <c r="B73" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D73" s="2">
-        <v>5</v>
-      </c>
-      <c r="E73" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="F73" s="2"/>
       <c r="G73" s="3" t="s">
-        <v>191</v>
+        <v>56</v>
       </c>
       <c r="H73" s="2"/>
     </row>
@@ -2545,53 +2548,53 @@
         <v>69</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D74" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>179</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D75" s="2">
-        <v>7</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>180</v>
-      </c>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
+      <c r="A76" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
+      <c r="G76" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="H76" s="2"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2599,20 +2602,20 @@
         <v>71</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>13</v>
+        <v>157</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2" t="s">
-        <v>199</v>
+      <c r="E77" s="2"/>
+      <c r="F77" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="H77" s="2"/>
     </row>
@@ -2621,136 +2624,136 @@
         <v>71</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>70</v>
+        <v>162</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="D78" s="2">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="3" t="s">
-        <v>86</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F78" s="3"/>
       <c r="G78" s="3" t="s">
-        <v>36</v>
+        <v>164</v>
       </c>
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D79" s="2">
-        <v>2</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3" t="s">
-        <v>165</v>
-      </c>
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="A80" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
+      <c r="G80" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2" t="s">
-        <v>81</v>
+      <c r="E81" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C82" s="2"/>
       <c r="D82" s="2">
         <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C83" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D83" s="2">
         <v>1</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
-      <c r="E84" s="3"/>
+      <c r="E84" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="H84" s="2"/>
     </row>
@@ -2759,21 +2762,19 @@
         <v>72</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>29</v>
+        <v>174</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="D85" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F85" s="3"/>
-      <c r="G85" s="3" t="s">
-        <v>177</v>
-      </c>
+      <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -2781,19 +2782,21 @@
         <v>72</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="D86" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F86" s="3"/>
-      <c r="G86" s="2"/>
+      <c r="G86" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -2801,20 +2804,20 @@
         <v>72</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>94</v>
+        <v>44</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D87" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F87" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="F87" s="2"/>
       <c r="G87" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H87" s="2"/>
     </row>
@@ -2823,20 +2826,18 @@
         <v>72</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>95</v>
+        <v>47</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="D88" s="2">
-        <v>4</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H88" s="2"/>
     </row>
@@ -2844,20 +2845,16 @@
       <c r="A89" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B89" s="2"/>
       <c r="C89" s="4" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="D89" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
-      <c r="G89" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="G89" s="3"/>
       <c r="H89" s="2"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -2877,275 +2874,259 @@
       <c r="H90" s="2"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="A91" s="2"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D91" s="2">
-        <v>2</v>
-      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="3"/>
+      <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
+      <c r="A92" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
+      <c r="G92" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="H92" s="2"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>74</v>
+        <v>167</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="D93" s="2">
         <v>1</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>82</v>
+      <c r="E93" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="F93" s="2"/>
-      <c r="G93" s="2" t="s">
-        <v>82</v>
+      <c r="G93" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="H93" s="2"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D94" s="2">
         <v>1</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H94" s="2"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>75</v>
+        <v>173</v>
       </c>
       <c r="D95" s="2">
         <v>1</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H96" s="2"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>172</v>
+        <v>77</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>173</v>
+        <v>76</v>
       </c>
       <c r="D97" s="2">
         <v>1</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="F97" s="2"/>
-      <c r="G97" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>76</v>
+        <v>192</v>
       </c>
       <c r="D98" s="2">
         <v>1</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="G98" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H98" s="2"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D99" s="2">
-        <v>1</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F99" s="2"/>
-      <c r="G99" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D100" s="7">
+        <v>184</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D99" s="7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A35:A41"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="A18:A27"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A47:A52"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="E59" r:id="rId1"/>
-    <hyperlink ref="G59" r:id="rId2"/>
-    <hyperlink ref="G79" r:id="rId3"/>
-    <hyperlink ref="E79" r:id="rId4"/>
-    <hyperlink ref="G60" r:id="rId5" location="prettyphoto/0/"/>
-    <hyperlink ref="G64" r:id="rId6"/>
-    <hyperlink ref="G65" r:id="rId7"/>
-    <hyperlink ref="G82" r:id="rId8"/>
-    <hyperlink ref="E82" r:id="rId9" display="SeedStudio"/>
-    <hyperlink ref="G83" r:id="rId10"/>
-    <hyperlink ref="E83" r:id="rId11"/>
-    <hyperlink ref="G84" r:id="rId12"/>
-    <hyperlink ref="E85" r:id="rId13"/>
-    <hyperlink ref="E87" r:id="rId14"/>
-    <hyperlink ref="G87" r:id="rId15"/>
-    <hyperlink ref="E67" r:id="rId16"/>
-    <hyperlink ref="G67" r:id="rId17"/>
-    <hyperlink ref="G70" r:id="rId18"/>
-    <hyperlink ref="E70" r:id="rId19"/>
-    <hyperlink ref="E88" r:id="rId20"/>
-    <hyperlink ref="G88" r:id="rId21"/>
-    <hyperlink ref="G89" r:id="rId22"/>
-    <hyperlink ref="G71" r:id="rId23"/>
-    <hyperlink ref="G72" r:id="rId24" display="wilco"/>
-    <hyperlink ref="G73" r:id="rId25"/>
-    <hyperlink ref="G74" r:id="rId26" display="wilco"/>
-    <hyperlink ref="G75" r:id="rId27" display="wilco"/>
-    <hyperlink ref="G62" r:id="rId28" location="prettyphoto/83/"/>
-    <hyperlink ref="G61" r:id="rId29"/>
-    <hyperlink ref="G95" r:id="rId30"/>
-    <hyperlink ref="E98" r:id="rId31"/>
-    <hyperlink ref="H98" r:id="rId32"/>
-    <hyperlink ref="H59" r:id="rId33"/>
-    <hyperlink ref="F59" r:id="rId34"/>
-    <hyperlink ref="G78" r:id="rId35"/>
-    <hyperlink ref="F78" r:id="rId36"/>
-    <hyperlink ref="G66" r:id="rId37" display="Amazon.jp"/>
-    <hyperlink ref="F62" r:id="rId38" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
-    <hyperlink ref="F61" r:id="rId39" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
-    <hyperlink ref="F60" r:id="rId40" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
-    <hyperlink ref="G63" r:id="rId41"/>
-    <hyperlink ref="E63" r:id="rId42"/>
-    <hyperlink ref="G85" r:id="rId43"/>
-    <hyperlink ref="E86" r:id="rId44"/>
-    <hyperlink ref="E72" r:id="rId45"/>
-    <hyperlink ref="E66" r:id="rId46"/>
-    <hyperlink ref="F66" r:id="rId47"/>
-    <hyperlink ref="H66" r:id="rId48"/>
-    <hyperlink ref="E94" r:id="rId49"/>
-    <hyperlink ref="G94" r:id="rId50"/>
-    <hyperlink ref="E96" r:id="rId51"/>
-    <hyperlink ref="E97" r:id="rId52"/>
-    <hyperlink ref="G96" r:id="rId53"/>
-    <hyperlink ref="G97" r:id="rId54"/>
-    <hyperlink ref="E95" r:id="rId55"/>
-    <hyperlink ref="E74" r:id="rId56"/>
-    <hyperlink ref="E75" r:id="rId57" display="Hirosugi-Keiki(SRU-2010)"/>
-    <hyperlink ref="F67" r:id="rId58" display="https://www.pololu.com/product/1058"/>
-    <hyperlink ref="G99" r:id="rId59"/>
-    <hyperlink ref="E99" r:id="rId60" display="Amaaon"/>
-    <hyperlink ref="G68" r:id="rId61"/>
-    <hyperlink ref="G69" r:id="rId62"/>
-    <hyperlink ref="E68" r:id="rId63"/>
-    <hyperlink ref="E69" r:id="rId64"/>
+    <hyperlink ref="E58" r:id="rId1"/>
+    <hyperlink ref="G58" r:id="rId2"/>
+    <hyperlink ref="G78" r:id="rId3"/>
+    <hyperlink ref="E78" r:id="rId4"/>
+    <hyperlink ref="G59" r:id="rId5" location="prettyphoto/0/"/>
+    <hyperlink ref="G63" r:id="rId6"/>
+    <hyperlink ref="G64" r:id="rId7"/>
+    <hyperlink ref="G81" r:id="rId8"/>
+    <hyperlink ref="E81" r:id="rId9" display="SeedStudio"/>
+    <hyperlink ref="G82" r:id="rId10"/>
+    <hyperlink ref="E82" r:id="rId11"/>
+    <hyperlink ref="G83" r:id="rId12"/>
+    <hyperlink ref="E84" r:id="rId13"/>
+    <hyperlink ref="E86" r:id="rId14"/>
+    <hyperlink ref="G86" r:id="rId15"/>
+    <hyperlink ref="E66" r:id="rId16"/>
+    <hyperlink ref="G66" r:id="rId17"/>
+    <hyperlink ref="G69" r:id="rId18"/>
+    <hyperlink ref="E69" r:id="rId19"/>
+    <hyperlink ref="E87" r:id="rId20"/>
+    <hyperlink ref="G87" r:id="rId21"/>
+    <hyperlink ref="G88" r:id="rId22"/>
+    <hyperlink ref="G70" r:id="rId23"/>
+    <hyperlink ref="G71" r:id="rId24" display="wilco"/>
+    <hyperlink ref="G72" r:id="rId25"/>
+    <hyperlink ref="G73" r:id="rId26" display="wilco"/>
+    <hyperlink ref="G74" r:id="rId27" display="wilco"/>
+    <hyperlink ref="G61" r:id="rId28" location="prettyphoto/83/"/>
+    <hyperlink ref="G60" r:id="rId29"/>
+    <hyperlink ref="G94" r:id="rId30"/>
+    <hyperlink ref="E97" r:id="rId31"/>
+    <hyperlink ref="H97" r:id="rId32"/>
+    <hyperlink ref="H58" r:id="rId33"/>
+    <hyperlink ref="F58" r:id="rId34"/>
+    <hyperlink ref="G77" r:id="rId35"/>
+    <hyperlink ref="F77" r:id="rId36"/>
+    <hyperlink ref="G65" r:id="rId37" display="Amazon.jp"/>
+    <hyperlink ref="F61" r:id="rId38" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
+    <hyperlink ref="F60" r:id="rId39" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
+    <hyperlink ref="F59" r:id="rId40" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
+    <hyperlink ref="G62" r:id="rId41"/>
+    <hyperlink ref="E62" r:id="rId42"/>
+    <hyperlink ref="G84" r:id="rId43"/>
+    <hyperlink ref="E85" r:id="rId44"/>
+    <hyperlink ref="E71" r:id="rId45"/>
+    <hyperlink ref="E65" r:id="rId46"/>
+    <hyperlink ref="F65" r:id="rId47"/>
+    <hyperlink ref="H65" r:id="rId48"/>
+    <hyperlink ref="E93" r:id="rId49"/>
+    <hyperlink ref="G93" r:id="rId50"/>
+    <hyperlink ref="E95" r:id="rId51"/>
+    <hyperlink ref="E96" r:id="rId52"/>
+    <hyperlink ref="G95" r:id="rId53"/>
+    <hyperlink ref="G96" r:id="rId54"/>
+    <hyperlink ref="E94" r:id="rId55"/>
+    <hyperlink ref="E73" r:id="rId56"/>
+    <hyperlink ref="E74" r:id="rId57" display="Hirosugi-Keiki(SRU-2010)"/>
+    <hyperlink ref="F66" r:id="rId58" display="https://www.pololu.com/product/1058"/>
+    <hyperlink ref="G98" r:id="rId59"/>
+    <hyperlink ref="E98" r:id="rId60" display="Amaaon"/>
+    <hyperlink ref="G67" r:id="rId61"/>
+    <hyperlink ref="G68" r:id="rId62"/>
+    <hyperlink ref="E67" r:id="rId63"/>
+    <hyperlink ref="E68" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId65"/>

</xml_diff>

<commit_message>
replace servo motor S03N with HD3001HB
</commit_message>
<xml_diff>
--- a/HACKberry-hardware/HACKberry_BOM_v1.xlsx
+++ b/HACKberry-hardware/HACKberry_BOM_v1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7575" tabRatio="589"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7572" tabRatio="589"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="199">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -171,10 +171,6 @@
   </si>
   <si>
     <t>US substitution</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>S03N</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -734,11 +730,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Pololu[3001HB]
-*haven't tested yet</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Lead Wire Cable 90mm</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -809,11 +800,19 @@
     <t>NA</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>HD3001HB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pololu</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -962,12 +961,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1009,7 +1011,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1044,7 +1046,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1256,24 +1258,24 @@
   <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.59765625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1285,24 +1287,24 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
@@ -1315,10 +1317,10 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -1331,10 +1333,10 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -1347,10 +1349,10 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1363,10 +1365,10 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1379,10 +1381,10 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -1395,10 +1397,10 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
@@ -1411,10 +1413,10 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1427,10 +1429,10 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
@@ -1443,10 +1445,10 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -1459,10 +1461,10 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>15</v>
@@ -1475,10 +1477,10 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>15</v>
@@ -1491,10 +1493,10 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
@@ -1507,10 +1509,10 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
@@ -1523,10 +1525,10 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>15</v>
@@ -1539,12 +1541,12 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>15</v>
@@ -1557,10 +1559,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>15</v>
@@ -1573,10 +1575,10 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
@@ -1589,10 +1591,10 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
@@ -1605,10 +1607,10 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>15</v>
@@ -1621,10 +1623,10 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>15</v>
@@ -1637,10 +1639,10 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>15</v>
@@ -1653,10 +1655,10 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
@@ -1669,10 +1671,10 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>15</v>
@@ -1685,10 +1687,10 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>15</v>
@@ -1701,12 +1703,12 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>15</v>
@@ -1719,10 +1721,10 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>15</v>
@@ -1735,10 +1737,10 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>15</v>
@@ -1751,10 +1753,10 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>15</v>
@@ -1767,10 +1769,10 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>15</v>
@@ -1783,10 +1785,10 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>15</v>
@@ -1799,10 +1801,10 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>15</v>
@@ -1815,12 +1817,12 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>15</v>
@@ -1831,10 +1833,10 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>15</v>
@@ -1845,10 +1847,10 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>15</v>
@@ -1859,10 +1861,10 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>15</v>
@@ -1873,10 +1875,10 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>15</v>
@@ -1887,10 +1889,10 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>15</v>
@@ -1901,10 +1903,10 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>15</v>
@@ -1915,9 +1917,9 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>3</v>
@@ -1933,7 +1935,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="2" t="s">
         <v>4</v>
@@ -1949,7 +1951,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
       <c r="B43" s="2" t="s">
         <v>5</v>
@@ -1965,7 +1967,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="2" t="s">
         <v>6</v>
@@ -1981,7 +1983,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
       <c r="B45" s="2" t="s">
         <v>7</v>
@@ -1997,12 +1999,12 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>15</v>
@@ -2015,12 +2017,12 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>15</v>
@@ -2033,10 +2035,10 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
       <c r="B48" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>15</v>
@@ -2049,10 +2051,10 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>15</v>
@@ -2065,10 +2067,10 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
       <c r="B50" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>15</v>
@@ -2081,10 +2083,10 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>15</v>
@@ -2097,10 +2099,10 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="10"/>
       <c r="B52" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>15</v>
@@ -2113,12 +2115,12 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>15</v>
@@ -2131,10 +2133,10 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
       <c r="B54" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>15</v>
@@ -2147,10 +2149,10 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="9"/>
       <c r="B55" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>15</v>
@@ -2163,10 +2165,10 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="10"/>
       <c r="B56" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>15</v>
@@ -2179,7 +2181,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2189,9 +2191,9 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>9</v>
@@ -2206,21 +2208,21 @@
         <v>10</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="66" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>17</v>
@@ -2230,88 +2232,88 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D60" s="2">
         <v>1</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C62" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62" s="2">
         <v>2</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D63" s="2">
         <v>25</v>
@@ -2323,9 +2325,9 @@
       </c>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>19</v>
@@ -2343,131 +2345,129 @@
       </c>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D65" s="2">
         <v>2</v>
       </c>
       <c r="E65" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="H65" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D66" s="2">
         <v>1</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E66" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F66" s="5"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="D67" s="2">
         <v>2</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="D69" s="2">
         <v>1</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D70" s="2">
         <v>46</v>
@@ -2479,37 +2479,37 @@
       </c>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D71" s="2">
         <v>6</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D72" s="2">
         <v>5</v>
@@ -2517,55 +2517,55 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D73" s="2">
         <v>10</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D74" s="2">
         <v>7</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2575,9 +2575,9 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>12</v>
@@ -2589,59 +2589,59 @@
         <v>1</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D77" s="2">
         <v>1</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="D78" s="2">
         <v>2</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2651,9 +2651,9 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>31</v>
@@ -2665,29 +2665,29 @@
         <v>1</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3" t="s">
@@ -2695,9 +2695,9 @@
       </c>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>23</v>
@@ -2715,9 +2715,9 @@
       </c>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>26</v>
@@ -2735,15 +2735,15 @@
       </c>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
@@ -2753,16 +2753,16 @@
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>33</v>
@@ -2777,15 +2777,15 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D86" s="2">
         <v>1</v>
@@ -2799,37 +2799,37 @@
       </c>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D87" s="2">
         <v>4</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H87" s="2"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C88" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
@@ -2837,17 +2837,17 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D89" s="2">
         <v>2</v>
@@ -2857,13 +2857,13 @@
       <c r="G89" s="3"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D90" s="2">
         <v>2</v>
@@ -2873,7 +2873,7 @@
       <c r="G90" s="3"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2883,169 +2883,169 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B92" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D92" s="2">
         <v>1</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H92" s="2"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
+      <c r="E93" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="D93" s="2">
-        <v>1</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
+      <c r="E94" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D94" s="2">
-        <v>1</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D95" s="2">
         <v>1</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D97" s="2">
         <v>1</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D98" s="2">
-        <v>1</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D99" s="7">
         <v>1</v>
@@ -3078,58 +3078,57 @@
     <hyperlink ref="E84" r:id="rId13"/>
     <hyperlink ref="E86" r:id="rId14"/>
     <hyperlink ref="G86" r:id="rId15"/>
-    <hyperlink ref="E66" r:id="rId16"/>
-    <hyperlink ref="G66" r:id="rId17"/>
-    <hyperlink ref="G69" r:id="rId18"/>
-    <hyperlink ref="E69" r:id="rId19"/>
-    <hyperlink ref="E87" r:id="rId20"/>
-    <hyperlink ref="G87" r:id="rId21"/>
-    <hyperlink ref="G88" r:id="rId22"/>
-    <hyperlink ref="G70" r:id="rId23"/>
-    <hyperlink ref="G71" r:id="rId24" display="wilco"/>
-    <hyperlink ref="G72" r:id="rId25"/>
-    <hyperlink ref="G73" r:id="rId26" display="wilco"/>
-    <hyperlink ref="G74" r:id="rId27" display="wilco"/>
-    <hyperlink ref="G61" r:id="rId28" location="prettyphoto/83/"/>
-    <hyperlink ref="G60" r:id="rId29"/>
-    <hyperlink ref="G94" r:id="rId30"/>
-    <hyperlink ref="E97" r:id="rId31"/>
-    <hyperlink ref="H97" r:id="rId32"/>
-    <hyperlink ref="H58" r:id="rId33"/>
-    <hyperlink ref="F58" r:id="rId34"/>
-    <hyperlink ref="G77" r:id="rId35"/>
-    <hyperlink ref="F77" r:id="rId36"/>
-    <hyperlink ref="G65" r:id="rId37" display="Amazon.jp"/>
-    <hyperlink ref="F61" r:id="rId38" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
-    <hyperlink ref="F60" r:id="rId39" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
-    <hyperlink ref="F59" r:id="rId40" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
-    <hyperlink ref="G62" r:id="rId41"/>
-    <hyperlink ref="E62" r:id="rId42"/>
-    <hyperlink ref="G84" r:id="rId43"/>
-    <hyperlink ref="E85" r:id="rId44"/>
-    <hyperlink ref="E71" r:id="rId45"/>
-    <hyperlink ref="E65" r:id="rId46"/>
-    <hyperlink ref="F65" r:id="rId47"/>
-    <hyperlink ref="H65" r:id="rId48"/>
-    <hyperlink ref="E93" r:id="rId49"/>
-    <hyperlink ref="G93" r:id="rId50"/>
-    <hyperlink ref="E95" r:id="rId51"/>
-    <hyperlink ref="E96" r:id="rId52"/>
-    <hyperlink ref="G95" r:id="rId53"/>
-    <hyperlink ref="G96" r:id="rId54"/>
-    <hyperlink ref="E94" r:id="rId55"/>
-    <hyperlink ref="E73" r:id="rId56"/>
-    <hyperlink ref="E74" r:id="rId57" display="Hirosugi-Keiki(SRU-2010)"/>
-    <hyperlink ref="F66" r:id="rId58" display="https://www.pololu.com/product/1058"/>
-    <hyperlink ref="G98" r:id="rId59"/>
-    <hyperlink ref="E98" r:id="rId60" display="Amaaon"/>
-    <hyperlink ref="G67" r:id="rId61"/>
-    <hyperlink ref="G68" r:id="rId62"/>
-    <hyperlink ref="E67" r:id="rId63"/>
-    <hyperlink ref="E68" r:id="rId64"/>
+    <hyperlink ref="G69" r:id="rId16"/>
+    <hyperlink ref="E69" r:id="rId17"/>
+    <hyperlink ref="E87" r:id="rId18"/>
+    <hyperlink ref="G87" r:id="rId19"/>
+    <hyperlink ref="G88" r:id="rId20"/>
+    <hyperlink ref="G70" r:id="rId21"/>
+    <hyperlink ref="G71" r:id="rId22" display="wilco"/>
+    <hyperlink ref="G72" r:id="rId23"/>
+    <hyperlink ref="G73" r:id="rId24" display="wilco"/>
+    <hyperlink ref="G74" r:id="rId25" display="wilco"/>
+    <hyperlink ref="G61" r:id="rId26" location="prettyphoto/83/"/>
+    <hyperlink ref="G60" r:id="rId27"/>
+    <hyperlink ref="G94" r:id="rId28"/>
+    <hyperlink ref="E97" r:id="rId29"/>
+    <hyperlink ref="H97" r:id="rId30"/>
+    <hyperlink ref="H58" r:id="rId31"/>
+    <hyperlink ref="F58" r:id="rId32"/>
+    <hyperlink ref="G77" r:id="rId33"/>
+    <hyperlink ref="F77" r:id="rId34"/>
+    <hyperlink ref="G65" r:id="rId35" display="Amazon.jp"/>
+    <hyperlink ref="F61" r:id="rId36" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType="/>
+    <hyperlink ref="F60" r:id="rId37" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType="/>
+    <hyperlink ref="F59" r:id="rId38" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType="/>
+    <hyperlink ref="G62" r:id="rId39"/>
+    <hyperlink ref="E62" r:id="rId40"/>
+    <hyperlink ref="G84" r:id="rId41"/>
+    <hyperlink ref="E85" r:id="rId42"/>
+    <hyperlink ref="E71" r:id="rId43"/>
+    <hyperlink ref="E65" r:id="rId44"/>
+    <hyperlink ref="F65" r:id="rId45"/>
+    <hyperlink ref="H65" r:id="rId46"/>
+    <hyperlink ref="E93" r:id="rId47"/>
+    <hyperlink ref="G93" r:id="rId48"/>
+    <hyperlink ref="E95" r:id="rId49"/>
+    <hyperlink ref="E96" r:id="rId50"/>
+    <hyperlink ref="G95" r:id="rId51"/>
+    <hyperlink ref="G96" r:id="rId52"/>
+    <hyperlink ref="E94" r:id="rId53"/>
+    <hyperlink ref="E73" r:id="rId54"/>
+    <hyperlink ref="E74" r:id="rId55" display="Hirosugi-Keiki(SRU-2010)"/>
+    <hyperlink ref="G98" r:id="rId56"/>
+    <hyperlink ref="E98" r:id="rId57" display="Amaaon"/>
+    <hyperlink ref="G67" r:id="rId58"/>
+    <hyperlink ref="G68" r:id="rId59"/>
+    <hyperlink ref="E67" r:id="rId60"/>
+    <hyperlink ref="E68" r:id="rId61"/>
+    <hyperlink ref="E66" r:id="rId62" display="https://www.pololu.com/product/1058"/>
+    <hyperlink ref="H66" r:id="rId63"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId65"/>
+  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId64"/>
 </worksheet>
 </file>
 
@@ -3139,7 +3138,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3152,7 +3151,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>